<commit_message>
historical employment and earnings
</commit_message>
<xml_diff>
--- a/data/historical/source/total_employment_historical.xlsx
+++ b/data/historical/source/total_employment_historical.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\RAuxier\Box Sync\TPC\CENTER\SLFI\SEM\Historical\Employment\PUBLISHED\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -178,13 +183,13 @@
     <t>United States</t>
   </si>
   <si>
-    <t>Total Employment; Year/Year: January 1990 -- February 2017</t>
+    <t>Total Employment; Year/Year: January 1990 -- May 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -204,40 +209,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -262,20 +267,20 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,6 +293,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -336,7 +344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,9 +377,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -404,6 +429,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -580,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA319"/>
+  <dimension ref="A1:BA322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E325" sqref="E325"/>
+      <selection pane="bottomLeft" activeCell="C321" sqref="C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -607,167 +649,167 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5" t="s">
+    <row r="4" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="5" t="s">
+      <c r="T5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="V5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="X5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y5" s="5" t="s">
+      <c r="Y5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA5" s="5" t="s">
+      <c r="AA5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AB5" s="5" t="s">
+      <c r="AB5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AC5" s="5" t="s">
+      <c r="AC5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="5" t="s">
+      <c r="AD5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AE5" s="5" t="s">
+      <c r="AE5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AF5" s="5" t="s">
+      <c r="AF5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AG5" s="5" t="s">
+      <c r="AG5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AH5" s="5" t="s">
+      <c r="AH5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AI5" s="5" t="s">
+      <c r="AI5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AJ5" s="5" t="s">
+      <c r="AJ5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AK5" s="5" t="s">
+      <c r="AK5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AL5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AM5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AN5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AO5" s="5" t="s">
+      <c r="AO5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AP5" s="5" t="s">
+      <c r="AP5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AQ5" s="5" t="s">
+      <c r="AQ5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AR5" s="5" t="s">
+      <c r="AR5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AS5" s="5" t="s">
+      <c r="AS5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AT5" s="5" t="s">
+      <c r="AT5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AU5" s="5" t="s">
+      <c r="AU5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AV5" s="5" t="s">
+      <c r="AV5" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AW5" s="5" t="s">
+      <c r="AW5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="AX5" s="5" t="s">
+      <c r="AX5" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AY5" s="5" t="s">
+      <c r="AY5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AZ5" s="5" t="s">
+      <c r="AZ5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="BA5" s="5" t="s">
+      <c r="BA5" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>33239</v>
       </c>
@@ -928,7 +970,7 @@
         <v>2.9141104294478617</v>
       </c>
     </row>
-    <row r="7" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>33270</v>
       </c>
@@ -1089,7 +1131,7 @@
         <v>2.9576746557878693</v>
       </c>
     </row>
-    <row r="8" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>33298</v>
       </c>
@@ -1250,7 +1292,7 @@
         <v>2.786220871327254</v>
       </c>
     </row>
-    <row r="9" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>33329</v>
       </c>
@@ -1411,7 +1453,7 @@
         <v>1.7042606516290755</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>33359</v>
       </c>
@@ -1572,7 +1614,7 @@
         <v>2.8340080971659893</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>33390</v>
       </c>
@@ -1733,7 +1775,7 @@
         <v>2.8297119757453233</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>33420</v>
       </c>
@@ -1894,7 +1936,7 @@
         <v>2.3761375126390232</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>33451</v>
       </c>
@@ -2055,7 +2097,7 @@
         <v>2.2635814889336014</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>33482</v>
       </c>
@@ -2216,7 +2258,7 @@
         <v>2.4635495223730546</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>33512</v>
       </c>
@@ -2377,7 +2419,7 @@
         <v>2.7094831911690802</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>33543</v>
       </c>
@@ -2538,7 +2580,7 @@
         <v>1.0923535253227352</v>
       </c>
     </row>
-    <row r="17" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>33573</v>
       </c>
@@ -2699,7 +2741,7 @@
         <v>1.3923421183490858</v>
       </c>
     </row>
-    <row r="18" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>33604</v>
       </c>
@@ -2860,7 +2902,7 @@
         <v>1.6890213611524973</v>
       </c>
     </row>
-    <row r="19" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>33635</v>
       </c>
@@ -3021,7 +3063,7 @@
         <v>1.4363546310054509</v>
       </c>
     </row>
-    <row r="20" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>33664</v>
       </c>
@@ -3182,7 +3224,7 @@
         <v>1.0842779694430698</v>
       </c>
     </row>
-    <row r="21" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>33695</v>
       </c>
@@ -3343,7 +3385,7 @@
         <v>0.73928043371118779</v>
       </c>
     </row>
-    <row r="22" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>33725</v>
       </c>
@@ -3504,7 +3546,7 @@
         <v>1.2795275590551294</v>
       </c>
     </row>
-    <row r="23" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>33756</v>
       </c>
@@ -3665,7 +3707,7 @@
         <v>0.49140049140049141</v>
       </c>
     </row>
-    <row r="24" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>33786</v>
       </c>
@@ -3826,7 +3868,7 @@
         <v>0.64197530864198094</v>
       </c>
     </row>
-    <row r="25" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>33817</v>
       </c>
@@ -3987,7 +4029,7 @@
         <v>1.5248401377274934</v>
       </c>
     </row>
-    <row r="26" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>33848</v>
       </c>
@@ -4148,7 +4190,7 @@
         <v>0.83415112855740359</v>
       </c>
     </row>
-    <row r="27" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>33878</v>
       </c>
@@ -4309,7 +4351,7 @@
         <v>0.92818759159746245</v>
       </c>
     </row>
-    <row r="28" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>33909</v>
       </c>
@@ -4470,7 +4512,7 @@
         <v>2.6522593320235788</v>
       </c>
     </row>
-    <row r="29" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>33939</v>
       </c>
@@ -4631,7 +4673,7 @@
         <v>1.4713094654242274</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>33970</v>
       </c>
@@ -4792,7 +4834,7 @@
         <v>1.5144113336590244</v>
       </c>
     </row>
-    <row r="31" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>34001</v>
       </c>
@@ -4953,7 +4995,7 @@
         <v>1.3183593749999944</v>
       </c>
     </row>
-    <row r="32" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>34029</v>
       </c>
@@ -5114,7 +5156,7 @@
         <v>1.3651877133105859</v>
       </c>
     </row>
-    <row r="33" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>34060</v>
       </c>
@@ -5275,7 +5317,7 @@
         <v>1.9569471624266144</v>
       </c>
     </row>
-    <row r="34" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>34090</v>
       </c>
@@ -5436,7 +5478,7 @@
         <v>1.6520894071914367</v>
       </c>
     </row>
-    <row r="35" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34121</v>
       </c>
@@ -5597,7 +5639,7 @@
         <v>2.9828850855745692</v>
       </c>
     </row>
-    <row r="36" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>34151</v>
       </c>
@@ -5758,7 +5800,7 @@
         <v>3.1894013738959761</v>
       </c>
     </row>
-    <row r="37" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>34182</v>
       </c>
@@ -5919,7 +5961,7 @@
         <v>2.4709302325581368</v>
       </c>
     </row>
-    <row r="38" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>34213</v>
       </c>
@@ -6080,7 +6122,7 @@
         <v>3.3090024330900296</v>
       </c>
     </row>
-    <row r="39" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>34243</v>
       </c>
@@ -6241,7 +6283,7 @@
         <v>2.9041626331074539</v>
       </c>
     </row>
-    <row r="40" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7">
         <v>34274</v>
       </c>
@@ -6402,7 +6444,7 @@
         <v>1.9138755980861244</v>
       </c>
     </row>
-    <row r="41" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>34304</v>
       </c>
@@ -6563,7 +6605,7 @@
         <v>3.4316094731754441</v>
       </c>
     </row>
-    <row r="42" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7">
         <v>34335</v>
       </c>
@@ -6724,7 +6766,7 @@
         <v>3.0317613089509061</v>
       </c>
     </row>
-    <row r="43" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>34366</v>
       </c>
@@ -6885,7 +6927,7 @@
         <v>3.2771084337349454</v>
       </c>
     </row>
-    <row r="44" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7">
         <v>34394</v>
       </c>
@@ -7046,7 +7088,7 @@
         <v>3.2708032708032624</v>
       </c>
     </row>
-    <row r="45" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>34425</v>
       </c>
@@ -7207,7 +7249,7 @@
         <v>3.4548944337811847</v>
       </c>
     </row>
-    <row r="46" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>34455</v>
       </c>
@@ -7368,7 +7410,7 @@
         <v>3.3938814531548864</v>
       </c>
     </row>
-    <row r="47" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>34486</v>
       </c>
@@ -7529,7 +7571,7 @@
         <v>2.5166191832858553</v>
       </c>
     </row>
-    <row r="48" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7">
         <v>34516</v>
       </c>
@@ -7690,7 +7732,7 @@
         <v>2.9006181645268638</v>
       </c>
     </row>
-    <row r="49" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>34547</v>
       </c>
@@ -7851,7 +7893,7 @@
         <v>4.0661938534278939</v>
       </c>
     </row>
-    <row r="50" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>34578</v>
       </c>
@@ -8012,7 +8054,7 @@
         <v>2.4964672633066334</v>
       </c>
     </row>
-    <row r="51" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>34608</v>
       </c>
@@ -8173,7 +8215,7 @@
         <v>2.492944496707437</v>
       </c>
     </row>
-    <row r="52" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>34639</v>
       </c>
@@ -8334,7 +8376,7 @@
         <v>3.4741784037558712</v>
       </c>
     </row>
-    <row r="53" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>34669</v>
       </c>
@@ -8495,7 +8537,7 @@
         <v>2.6635514018691535</v>
       </c>
     </row>
-    <row r="54" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>34700</v>
       </c>
@@ -8656,7 +8698,7 @@
         <v>2.3820644558617441</v>
       </c>
     </row>
-    <row r="55" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>34731</v>
       </c>
@@ -8817,7 +8859,7 @@
         <v>2.4265048996733496</v>
       </c>
     </row>
-    <row r="56" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>34759</v>
       </c>
@@ -8978,7 +9020,7 @@
         <v>2.3288309268747089</v>
       </c>
     </row>
-    <row r="57" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>34790</v>
       </c>
@@ -9139,7 +9181,7 @@
         <v>1.7161410018552956</v>
       </c>
     </row>
-    <row r="58" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>34820</v>
       </c>
@@ -9300,7 +9342,7 @@
         <v>0.92464170134073043</v>
       </c>
     </row>
-    <row r="59" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>34851</v>
       </c>
@@ -9461,7 +9503,7 @@
         <v>1.9916628068550175</v>
       </c>
     </row>
-    <row r="60" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>34881</v>
       </c>
@@ -9622,7 +9664,7 @@
         <v>0.41589648798521517</v>
       </c>
     </row>
-    <row r="61" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>34912</v>
       </c>
@@ -9783,7 +9825,7 @@
         <v>-0.95411176737846182</v>
       </c>
     </row>
-    <row r="62" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>34943</v>
       </c>
@@ -9944,7 +9986,7 @@
         <v>1.1488970588235294</v>
       </c>
     </row>
-    <row r="63" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>34973</v>
       </c>
@@ -10105,7 +10147,7 @@
         <v>1.1932078935291393</v>
       </c>
     </row>
-    <row r="64" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>35004</v>
       </c>
@@ -10266,7 +10308,7 @@
         <v>-0.40834845735027481</v>
       </c>
     </row>
-    <row r="65" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="7">
         <v>35034</v>
       </c>
@@ -10427,7 +10469,7 @@
         <v>0.22758306781975424</v>
       </c>
     </row>
-    <row r="66" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="7">
         <v>35065</v>
       </c>
@@ -10588,7 +10630,7 @@
         <v>0.45620437956204385</v>
       </c>
     </row>
-    <row r="67" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>35096</v>
       </c>
@@ -10749,7 +10791,7 @@
         <v>0.5011389521640065</v>
       </c>
     </row>
-    <row r="68" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="7">
         <v>35125</v>
       </c>
@@ -10910,7 +10952,7 @@
         <v>9.1033227127909455E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7">
         <v>35156</v>
       </c>
@@ -11071,7 +11113,7 @@
         <v>0.68399452804377558</v>
       </c>
     </row>
-    <row r="70" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="7">
         <v>35186</v>
       </c>
@@ -11232,7 +11274,7 @@
         <v>1.3284470911589452</v>
       </c>
     </row>
-    <row r="71" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="7">
         <v>35217</v>
       </c>
@@ -11393,7 +11435,7 @@
         <v>0.72661217075387052</v>
       </c>
     </row>
-    <row r="72" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="7">
         <v>35247</v>
       </c>
@@ -11554,7 +11596,7 @@
         <v>0.87436723423836948</v>
       </c>
     </row>
-    <row r="73" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="7">
         <v>35278</v>
       </c>
@@ -11715,7 +11757,7 @@
         <v>1.651376146788988</v>
       </c>
     </row>
-    <row r="74" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="7">
         <v>35309</v>
       </c>
@@ -11876,7 +11918,7 @@
         <v>0.95411176737846182</v>
       </c>
     </row>
-    <row r="75" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="7">
         <v>35339</v>
       </c>
@@ -12037,7 +12079,7 @@
         <v>0.90702947845804993</v>
       </c>
     </row>
-    <row r="76" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="7">
         <v>35370</v>
       </c>
@@ -12198,7 +12240,7 @@
         <v>1.6856492027334802</v>
       </c>
     </row>
-    <row r="77" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="7">
         <v>35400</v>
       </c>
@@ -12359,7 +12401,7 @@
         <v>0.49954586739328916</v>
       </c>
     </row>
-    <row r="78" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="7">
         <v>35431</v>
       </c>
@@ -12520,7 +12562,7 @@
         <v>0.72661217075387052</v>
       </c>
     </row>
-    <row r="79" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="7">
         <v>35462</v>
       </c>
@@ -12681,7 +12723,7 @@
         <v>0.54397098821396961</v>
       </c>
     </row>
-    <row r="80" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="7">
         <v>35490</v>
       </c>
@@ -12842,7 +12884,7 @@
         <v>1.1368804001819008</v>
       </c>
     </row>
-    <row r="81" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="7">
         <v>35521</v>
       </c>
@@ -13003,7 +13045,7 @@
         <v>1.1775362318840554</v>
       </c>
     </row>
-    <row r="82" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="7">
         <v>35551</v>
       </c>
@@ -13164,7 +13206,7 @@
         <v>1.4918625678119402</v>
       </c>
     </row>
-    <row r="83" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="7">
         <v>35582</v>
       </c>
@@ -13325,7 +13367,7 @@
         <v>1.0820559062218111</v>
       </c>
     </row>
-    <row r="84" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>35612</v>
       </c>
@@ -13486,7 +13528,7 @@
         <v>2.8284671532846795</v>
       </c>
     </row>
-    <row r="85" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="7">
         <v>35643</v>
       </c>
@@ -13647,7 +13689,7 @@
         <v>1.895306859205784</v>
       </c>
     </row>
-    <row r="86" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="7">
         <v>35674</v>
       </c>
@@ -13808,7 +13850,7 @@
         <v>1.8001800180018002</v>
       </c>
     </row>
-    <row r="87" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="7">
         <v>35704</v>
       </c>
@@ -13969,7 +14011,7 @@
         <v>1.7078651685393309</v>
       </c>
     </row>
-    <row r="88" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="7">
         <v>35735</v>
       </c>
@@ -14130,7 +14172,7 @@
         <v>1.4784946236559191</v>
       </c>
     </row>
-    <row r="89" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="7">
         <v>35765</v>
       </c>
@@ -14291,7 +14333,7 @@
         <v>2.6208766380478909</v>
       </c>
     </row>
-    <row r="90" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="7">
         <v>35796</v>
       </c>
@@ -14452,7 +14494,7 @@
         <v>2.3895401262398477</v>
       </c>
     </row>
-    <row r="91" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="7">
         <v>35827</v>
       </c>
@@ -14613,7 +14655,7 @@
         <v>2.6600541027953009</v>
       </c>
     </row>
-    <row r="92" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="7">
         <v>35855</v>
       </c>
@@ -14774,7 +14816,7 @@
         <v>2.0233812949640289</v>
       </c>
     </row>
-    <row r="93" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>35886</v>
       </c>
@@ -14935,7 +14977,7 @@
         <v>1.8352730528200512</v>
       </c>
     </row>
-    <row r="94" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="7">
         <v>35916</v>
       </c>
@@ -15096,7 +15138,7 @@
         <v>2.4498886414253898</v>
       </c>
     </row>
-    <row r="95" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="7">
         <v>35947</v>
       </c>
@@ -15257,7 +15299,7 @@
         <v>1.6949152542372934</v>
       </c>
     </row>
-    <row r="96" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="7">
         <v>35977</v>
       </c>
@@ -15418,7 +15460,7 @@
         <v>0.9316770186335378</v>
       </c>
     </row>
-    <row r="97" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="7">
         <v>36008</v>
       </c>
@@ -15579,7 +15621,7 @@
         <v>0.93002657218777418</v>
       </c>
     </row>
-    <row r="98" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7">
         <v>36039</v>
       </c>
@@ -15740,7 +15782,7 @@
         <v>1.0167992926613667</v>
       </c>
     </row>
-    <row r="99" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="7">
         <v>36069</v>
       </c>
@@ -15901,7 +15943,7 @@
         <v>1.1489173663278807</v>
       </c>
     </row>
-    <row r="100" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="7">
         <v>36100</v>
       </c>
@@ -16062,7 +16104,7 @@
         <v>1.5894039735099312</v>
       </c>
     </row>
-    <row r="101" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="7">
         <v>36130</v>
       </c>
@@ -16223,7 +16265,7 @@
         <v>1.3650374284456162</v>
       </c>
     </row>
-    <row r="102" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="7">
         <v>36161</v>
       </c>
@@ -16384,7 +16426,7 @@
         <v>1.3650374284456162</v>
       </c>
     </row>
-    <row r="103" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="7">
         <v>36192</v>
       </c>
@@ -16545,7 +16587,7 @@
         <v>1.1857707509881499</v>
       </c>
     </row>
-    <row r="104" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="7">
         <v>36220</v>
       </c>
@@ -16706,7 +16748,7 @@
         <v>2.1595416483032195</v>
       </c>
     </row>
-    <row r="105" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="7">
         <v>36251</v>
       </c>
@@ -16867,7 +16909,7 @@
         <v>1.9340659340659365</v>
       </c>
     </row>
-    <row r="106" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="7">
         <v>36281</v>
       </c>
@@ -17028,7 +17070,7 @@
         <v>1.1304347826086933</v>
       </c>
     </row>
-    <row r="107" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="7">
         <v>36312</v>
       </c>
@@ -17189,7 +17231,7 @@
         <v>2.1052631578947421</v>
       </c>
     </row>
-    <row r="108" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="7">
         <v>36342</v>
       </c>
@@ -17350,7 +17392,7 @@
         <v>2.6373626373626373</v>
       </c>
     </row>
-    <row r="109" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="7">
         <v>36373</v>
       </c>
@@ -17511,7 +17553,7 @@
         <v>2.4572180781044293</v>
       </c>
     </row>
-    <row r="110" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="7">
         <v>36404</v>
       </c>
@@ -17672,7 +17714,7 @@
         <v>2.6695842450765839</v>
       </c>
     </row>
-    <row r="111" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="7">
         <v>36434</v>
       </c>
@@ -17833,7 +17875,7 @@
         <v>2.7086063783311443</v>
       </c>
     </row>
-    <row r="112" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="7">
         <v>36465</v>
       </c>
@@ -17994,7 +18036,7 @@
         <v>2.4337244676227705</v>
       </c>
     </row>
-    <row r="113" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="7">
         <v>36495</v>
       </c>
@@ -18155,7 +18197,7 @@
         <v>2.7801911381407498</v>
       </c>
     </row>
-    <row r="114" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="7">
         <v>36526</v>
       </c>
@@ -18316,7 +18358,7 @@
         <v>3.0842745438749013</v>
       </c>
     </row>
-    <row r="115" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="7">
         <v>36557</v>
       </c>
@@ -18477,7 +18519,7 @@
         <v>3.3854166666666594</v>
       </c>
     </row>
-    <row r="116" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="7">
         <v>36586</v>
       </c>
@@ -18638,7 +18680,7 @@
         <v>3.4081104400345024</v>
       </c>
     </row>
-    <row r="117" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="7">
         <v>36617</v>
       </c>
@@ -18799,7 +18841,7 @@
         <v>3.2341526520051747</v>
       </c>
     </row>
-    <row r="118" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="7">
         <v>36647</v>
       </c>
@@ -18960,7 +19002,7 @@
         <v>2.9234737747205553</v>
       </c>
     </row>
-    <row r="119" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="7">
         <v>36678</v>
       </c>
@@ -19121,7 +19163,7 @@
         <v>2.0189003436426067</v>
       </c>
     </row>
-    <row r="120" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="7">
         <v>36708</v>
       </c>
@@ -19282,7 +19324,7 @@
         <v>2.441113490364021</v>
       </c>
     </row>
-    <row r="121" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="7">
         <v>36739</v>
       </c>
@@ -19443,7 +19485,7 @@
         <v>2.9978586723768736</v>
       </c>
     </row>
-    <row r="122" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="7">
         <v>36770</v>
       </c>
@@ -19604,7 +19646,7 @@
         <v>1.9607843137254877</v>
       </c>
     </row>
-    <row r="123" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="7">
         <v>36800</v>
       </c>
@@ -19765,7 +19807,7 @@
         <v>2.2543598468736756</v>
       </c>
     </row>
-    <row r="124" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="7">
         <v>36831</v>
       </c>
@@ -19926,7 +19968,7 @@
         <v>1.9516334323292417</v>
       </c>
     </row>
-    <row r="125" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="7">
         <v>36861</v>
       </c>
@@ -20087,7 +20129,7 @@
         <v>2.1132713440405748</v>
       </c>
     </row>
-    <row r="126" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="7">
         <v>36892</v>
       </c>
@@ -20248,7 +20290,7 @@
         <v>2.2334597555836422</v>
       </c>
     </row>
-    <row r="127" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="7">
         <v>36923</v>
       </c>
@@ -20409,7 +20451,7 @@
         <v>2.2250209907640688</v>
       </c>
     </row>
-    <row r="128" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="7">
         <v>36951</v>
       </c>
@@ -20570,7 +20612,7 @@
         <v>1.8356278681685465</v>
       </c>
     </row>
-    <row r="129" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="7">
         <v>36982</v>
       </c>
@@ -20731,7 +20773,7 @@
         <v>2.1303258145363384</v>
       </c>
     </row>
-    <row r="130" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="7">
         <v>37012</v>
       </c>
@@ -20892,7 +20934,7 @@
         <v>2.4227234753550473</v>
       </c>
     </row>
-    <row r="131" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131" s="7">
         <v>37043</v>
       </c>
@@ -21053,7 +21095,7 @@
         <v>3.1999999999999975</v>
       </c>
     </row>
-    <row r="132" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="7">
         <v>37073</v>
       </c>
@@ -21214,7 +21256,7 @@
         <v>2.7173913043478262</v>
       </c>
     </row>
-    <row r="133" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="7">
         <v>37104</v>
       </c>
@@ -21375,7 +21417,7 @@
         <v>2.7858627858627814</v>
       </c>
     </row>
-    <row r="134" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="7">
         <v>37135</v>
       </c>
@@ -21536,7 +21578,7 @@
         <v>2.7173913043478262</v>
       </c>
     </row>
-    <row r="135" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="7">
         <v>37165</v>
       </c>
@@ -21697,7 +21739,7 @@
         <v>2.4958402662229617</v>
       </c>
     </row>
-    <row r="136" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="7">
         <v>37196</v>
       </c>
@@ -21858,7 +21900,7 @@
         <v>3.0378693300041544</v>
       </c>
     </row>
-    <row r="137" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="7">
         <v>37226</v>
       </c>
@@ -22019,7 +22061,7 @@
         <v>2.4834437086092715</v>
       </c>
     </row>
-    <row r="138" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="7">
         <v>37257</v>
       </c>
@@ -22180,7 +22222,7 @@
         <v>1.9373454245671959</v>
       </c>
     </row>
-    <row r="139" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="7">
         <v>37288</v>
       </c>
@@ -22341,7 +22383,7 @@
         <v>1.6427104722792609</v>
       </c>
     </row>
-    <row r="140" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="7">
         <v>37316</v>
       </c>
@@ -22502,7 +22544,7 @@
         <v>1.3109381401065208</v>
       </c>
     </row>
-    <row r="141" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="7">
         <v>37347</v>
       </c>
@@ -22663,7 +22705,7 @@
         <v>1.2269938650306749</v>
       </c>
     </row>
-    <row r="142" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="7">
         <v>37377</v>
       </c>
@@ -22824,7 +22866,7 @@
         <v>1.1827079934747169</v>
       </c>
     </row>
-    <row r="143" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="7">
         <v>37408</v>
       </c>
@@ -22985,7 +23027,7 @@
         <v>1.1015911872705089</v>
       </c>
     </row>
-    <row r="144" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="7">
         <v>37438</v>
       </c>
@@ -23146,7 +23188,7 @@
         <v>1.0175010175010175</v>
       </c>
     </row>
-    <row r="145" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="7">
         <v>37469</v>
       </c>
@@ -23307,7 +23349,7 @@
         <v>0.28317152103560561</v>
       </c>
     </row>
-    <row r="146" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="7">
         <v>37500</v>
       </c>
@@ -23468,7 +23510,7 @@
         <v>1.2210012210012211</v>
       </c>
     </row>
-    <row r="147" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="7">
         <v>37530</v>
       </c>
@@ -23629,7 +23671,7 @@
         <v>0.73051948051947357</v>
       </c>
     </row>
-    <row r="148" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="7">
         <v>37561</v>
       </c>
@@ -23790,7 +23832,7 @@
         <v>0.36348949919224788</v>
       </c>
     </row>
-    <row r="149" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="7">
         <v>37591</v>
       </c>
@@ -23951,7 +23993,7 @@
         <v>0.32310177705977844</v>
       </c>
     </row>
-    <row r="150" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="7">
         <v>37622</v>
       </c>
@@ -24112,7 +24154,7 @@
         <v>0.36393044884754433</v>
       </c>
     </row>
-    <row r="151" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="7">
         <v>37653</v>
       </c>
@@ -24273,7 +24315,7 @@
         <v>0.12121212121212581</v>
       </c>
     </row>
-    <row r="152" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="7">
         <v>37681</v>
       </c>
@@ -24434,7 +24476,7 @@
         <v>-0.16174686615447054</v>
       </c>
     </row>
-    <row r="153" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153" s="7">
         <v>37712</v>
       </c>
@@ -24595,7 +24637,7 @@
         <v>0.24242424242424013</v>
       </c>
     </row>
-    <row r="154" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
         <v>37742</v>
       </c>
@@ -24756,7 +24798,7 @@
         <v>0.24183796856106182</v>
       </c>
     </row>
-    <row r="155" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
         <v>37773</v>
       </c>
@@ -24917,7 +24959,7 @@
         <v>0.88781275221952727</v>
       </c>
     </row>
-    <row r="156" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="7">
         <v>37803</v>
       </c>
@@ -25078,7 +25120,7 @@
         <v>0.76551168412570747</v>
       </c>
     </row>
-    <row r="157" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157" s="7">
         <v>37834</v>
       </c>
@@ -25239,7 +25281,7 @@
         <v>1.4118596208148446</v>
       </c>
     </row>
-    <row r="158" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
         <v>37865</v>
       </c>
@@ -25400,7 +25442,7 @@
         <v>1.36710896662646</v>
       </c>
     </row>
-    <row r="159" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
         <v>37895</v>
       </c>
@@ -25561,7 +25603,7 @@
         <v>1.8936341659951721</v>
       </c>
     </row>
-    <row r="160" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
         <v>37926</v>
       </c>
@@ -25722,7 +25764,7 @@
         <v>1.5291750503018156</v>
       </c>
     </row>
-    <row r="161" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
         <v>37956</v>
       </c>
@@ -25883,7 +25925,7 @@
         <v>1.6908212560386426</v>
       </c>
     </row>
-    <row r="162" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
         <v>37987</v>
       </c>
@@ -26044,7 +26086,7 @@
         <v>2.0547945205479543</v>
       </c>
     </row>
-    <row r="163" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163" s="7">
         <v>38018</v>
       </c>
@@ -26205,7 +26247,7 @@
         <v>2.2195318805488298</v>
       </c>
     </row>
-    <row r="164" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164" s="7">
         <v>38047</v>
       </c>
@@ -26366,7 +26408,7 @@
         <v>2.7946537059538299</v>
       </c>
     </row>
-    <row r="165" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="7">
         <v>38078</v>
       </c>
@@ -26527,7 +26569,7 @@
         <v>2.9020556227327758</v>
       </c>
     </row>
-    <row r="166" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166" s="7">
         <v>38108</v>
       </c>
@@ -26688,7 +26730,7 @@
         <v>2.3321270607157265</v>
       </c>
     </row>
-    <row r="167" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167" s="7">
         <v>38139</v>
       </c>
@@ -26849,7 +26891,7 @@
         <v>2.239999999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="7">
         <v>38169</v>
       </c>
@@ -27010,7 +27052,7 @@
         <v>2.3190723710515839</v>
       </c>
     </row>
-    <row r="169" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
         <v>38200</v>
       </c>
@@ -27171,7 +27213,7 @@
         <v>1.9093078758949813</v>
       </c>
     </row>
-    <row r="170" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
         <v>38231</v>
       </c>
@@ -27332,7 +27374,7 @@
         <v>1.1503371677905616</v>
       </c>
     </row>
-    <row r="171" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
         <v>38261</v>
       </c>
@@ -27493,7 +27535,7 @@
         <v>1.4234875444839834</v>
       </c>
     </row>
-    <row r="172" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
         <v>38292</v>
       </c>
@@ -27654,7 +27696,7 @@
         <v>2.1799445105033692</v>
       </c>
     </row>
-    <row r="173" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
         <v>38322</v>
       </c>
@@ -27815,7 +27857,7 @@
         <v>2.2169437846397444</v>
       </c>
     </row>
-    <row r="174" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
         <v>38353</v>
       </c>
@@ -27976,7 +28018,7 @@
         <v>2.1318594551914636</v>
       </c>
     </row>
-    <row r="175" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
         <v>38384</v>
       </c>
@@ -28137,7 +28179,7 @@
         <v>2.4476904855902046</v>
       </c>
     </row>
-    <row r="176" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
         <v>38412</v>
       </c>
@@ -28298,7 +28340,7 @@
         <v>2.8368794326241087</v>
       </c>
     </row>
-    <row r="177" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
         <v>38443</v>
       </c>
@@ -28459,7 +28501,7 @@
         <v>2.5460242851547199</v>
       </c>
     </row>
-    <row r="178" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178" s="7">
         <v>38473</v>
       </c>
@@ -28620,7 +28662,7 @@
         <v>3.0648330058939139</v>
       </c>
     </row>
-    <row r="179" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
         <v>38504</v>
       </c>
@@ -28781,7 +28823,7 @@
         <v>2.5821596244131433</v>
       </c>
     </row>
-    <row r="180" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
         <v>38534</v>
       </c>
@@ -28942,7 +28984,7 @@
         <v>3.3606877686596301</v>
       </c>
     </row>
-    <row r="181" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
         <v>38565</v>
       </c>
@@ -29103,7 +29145,7 @@
         <v>3.8251366120218631</v>
       </c>
     </row>
-    <row r="182" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182" s="7">
         <v>38596</v>
       </c>
@@ -29264,7 +29306,7 @@
         <v>4.5098039215686274</v>
       </c>
     </row>
-    <row r="183" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183" s="7">
         <v>38626</v>
       </c>
@@ -29425,7 +29467,7 @@
         <v>4.2884990253411299</v>
       </c>
     </row>
-    <row r="184" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
         <v>38657</v>
       </c>
@@ -29586,7 +29628,7 @@
         <v>4.0729247478665629</v>
       </c>
     </row>
-    <row r="185" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
         <v>38687</v>
       </c>
@@ -29747,7 +29789,7 @@
         <v>4.2602633617350891</v>
       </c>
     </row>
-    <row r="186" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
         <v>38718</v>
       </c>
@@ -29908,7 +29950,7 @@
         <v>4.9478160030923899</v>
       </c>
     </row>
-    <row r="187" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
         <v>38749</v>
       </c>
@@ -30069,7 +30111,7 @@
         <v>5.1252408477842053</v>
       </c>
     </row>
-    <row r="188" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
         <v>38777</v>
       </c>
@@ -30230,7 +30272,7 @@
         <v>5.0574712643678117</v>
       </c>
     </row>
-    <row r="189" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
         <v>38808</v>
       </c>
@@ -30391,7 +30433,7 @@
         <v>5.2330022918258168</v>
       </c>
     </row>
-    <row r="190" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
         <v>38838</v>
       </c>
@@ -30552,7 +30594,7 @@
         <v>5.4136484940907312</v>
       </c>
     </row>
-    <row r="191" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
         <v>38869</v>
       </c>
@@ -30713,7 +30755,7 @@
         <v>5.8352402745995473</v>
       </c>
     </row>
-    <row r="192" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192" s="7">
         <v>38899</v>
       </c>
@@ -30874,7 +30916,7 @@
         <v>4.9149338374291114</v>
       </c>
     </row>
-    <row r="193" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193" s="7">
         <v>38930</v>
       </c>
@@ -31035,7 +31077,7 @@
         <v>4.9248120300751967</v>
       </c>
     </row>
-    <row r="194" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194" s="7">
         <v>38961</v>
       </c>
@@ -31196,7 +31238,7 @@
         <v>4.9155722326454123</v>
       </c>
     </row>
-    <row r="195" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195" s="7">
         <v>38991</v>
       </c>
@@ -31357,7 +31399,7 @@
         <v>4.6728971962616823</v>
       </c>
     </row>
-    <row r="196" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196" s="7">
         <v>39022</v>
       </c>
@@ -31518,7 +31560,7 @@
         <v>4.7707789787551285</v>
       </c>
     </row>
-    <row r="197" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197" s="7">
         <v>39052</v>
       </c>
@@ -31679,7 +31721,7 @@
         <v>5.3863298662704313</v>
       </c>
     </row>
-    <row r="198" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="7">
         <v>39083</v>
       </c>
@@ -31840,7 +31882,7 @@
         <v>4.8987108655616982</v>
       </c>
     </row>
-    <row r="199" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="7">
         <v>39114</v>
       </c>
@@ -32001,7 +32043,7 @@
         <v>4.7287390029325431</v>
       </c>
     </row>
-    <row r="200" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="7">
         <v>39142</v>
       </c>
@@ -32162,7 +32204,7 @@
         <v>4.7410649161196208</v>
       </c>
     </row>
-    <row r="201" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201" s="7">
         <v>39173</v>
       </c>
@@ -32323,7 +32365,7 @@
         <v>4.13793103448275</v>
       </c>
     </row>
-    <row r="202" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202" s="7">
         <v>39203</v>
       </c>
@@ -32484,7 +32526,7 @@
         <v>4.1229656419529759</v>
       </c>
     </row>
-    <row r="203" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203" s="7">
         <v>39234</v>
       </c>
@@ -32645,7 +32687,7 @@
         <v>3.855855855855852</v>
       </c>
     </row>
-    <row r="204" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204" s="7">
         <v>39264</v>
       </c>
@@ -32806,7 +32848,7 @@
         <v>4.1801801801801881</v>
       </c>
     </row>
-    <row r="205" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205" s="7">
         <v>39295</v>
       </c>
@@ -32967,7 +33009,7 @@
         <v>3.7262629881762726</v>
       </c>
     </row>
-    <row r="206" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206" s="7">
         <v>39326</v>
       </c>
@@ -33128,7 +33170,7 @@
         <v>3.7911301859799589</v>
       </c>
     </row>
-    <row r="207" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207" s="7">
         <v>39356</v>
       </c>
@@ -33289,7 +33331,7 @@
         <v>4.03571428571429</v>
       </c>
     </row>
-    <row r="208" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208" s="7">
         <v>39387</v>
       </c>
@@ -33450,7 +33492,7 @@
         <v>4.3045179651369496</v>
       </c>
     </row>
-    <row r="209" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209" s="7">
         <v>39417</v>
       </c>
@@ -33611,7 +33653,7 @@
         <v>3.7363412054987744</v>
       </c>
     </row>
-    <row r="210" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210" s="7">
         <v>39448</v>
       </c>
@@ -33772,7 +33814,7 @@
         <v>3.8623595505617976</v>
       </c>
     </row>
-    <row r="211" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211" s="7">
         <v>39479</v>
       </c>
@@ -33933,7 +33975,7 @@
         <v>3.7801890094504769</v>
       </c>
     </row>
-    <row r="212" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212" s="7">
         <v>39508</v>
       </c>
@@ -34094,7 +34136,7 @@
         <v>3.3077994428969362</v>
       </c>
     </row>
-    <row r="213" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213" s="7">
         <v>39539</v>
       </c>
@@ -34255,7 +34297,7 @@
         <v>3.485535029627048</v>
       </c>
     </row>
-    <row r="214" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214" s="7">
         <v>39569</v>
       </c>
@@ -34416,7 +34458,7 @@
         <v>3.5081625564432173</v>
       </c>
     </row>
-    <row r="215" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215" s="7">
         <v>39600</v>
       </c>
@@ -34577,7 +34619,7 @@
         <v>3.3657182512144308</v>
       </c>
     </row>
-    <row r="216" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="7">
         <v>39630</v>
       </c>
@@ -34738,7 +34780,7 @@
         <v>3.2514700795572384</v>
       </c>
     </row>
-    <row r="217" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217" s="7">
         <v>39661</v>
       </c>
@@ -34899,7 +34941,7 @@
         <v>3.0051813471502551</v>
       </c>
     </row>
-    <row r="218" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218" s="7">
         <v>39692</v>
       </c>
@@ -35060,7 +35102,7 @@
         <v>3.032391454169542</v>
       </c>
     </row>
-    <row r="219" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219" s="7">
         <v>39722</v>
       </c>
@@ -35221,7 +35263,7 @@
         <v>2.9179539993134225</v>
       </c>
     </row>
-    <row r="220" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220" s="7">
         <v>39753</v>
       </c>
@@ -35382,7 +35424,7 @@
         <v>2.0122783083219762</v>
       </c>
     </row>
-    <row r="221" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221" s="7">
         <v>39783</v>
       </c>
@@ -35543,7 +35585,7 @@
         <v>1.1213047910295655</v>
       </c>
     </row>
-    <row r="222" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222" s="7">
         <v>39814</v>
       </c>
@@ -35704,7 +35746,7 @@
         <v>-0.23664638269100358</v>
       </c>
     </row>
-    <row r="223" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223" s="7">
         <v>39845</v>
       </c>
@@ -35865,7 +35907,7 @@
         <v>-1.2141652613828069</v>
       </c>
     </row>
-    <row r="224" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224" s="7">
         <v>39873</v>
       </c>
@@ -36026,7 +36068,7 @@
         <v>-1.9211324570272965</v>
       </c>
     </row>
-    <row r="225" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225" s="7">
         <v>39904</v>
       </c>
@@ -36187,7 +36229,7 @@
         <v>-3.0313236780060628</v>
       </c>
     </row>
-    <row r="226" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226" s="7">
         <v>39934</v>
       </c>
@@ -36348,7 +36390,7 @@
         <v>-3.087248322147647</v>
       </c>
     </row>
-    <row r="227" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227" s="7">
         <v>39965</v>
       </c>
@@ -36509,7 +36551,7 @@
         <v>-4.2631755622692138</v>
       </c>
     </row>
-    <row r="228" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228" s="7">
         <v>39995</v>
       </c>
@@ -36670,7 +36712,7 @@
         <v>-5.025125628140704</v>
       </c>
     </row>
-    <row r="229" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" s="7">
         <v>40026</v>
       </c>
@@ -36831,7 +36873,7 @@
         <v>-5.3990610328638393</v>
       </c>
     </row>
-    <row r="230" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230" s="7">
         <v>40057</v>
       </c>
@@ -36992,7 +37034,7 @@
         <v>-5.4515050167224119</v>
       </c>
     </row>
-    <row r="231" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A231" s="7">
         <v>40087</v>
       </c>
@@ -37153,7 +37195,7 @@
         <v>-6.3709139426284267</v>
       </c>
     </row>
-    <row r="232" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A232" s="7">
         <v>40118</v>
       </c>
@@ -37314,7 +37356,7 @@
         <v>-6.2186559679037181</v>
       </c>
     </row>
-    <row r="233" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A233" s="7">
         <v>40148</v>
       </c>
@@ -37475,7 +37517,7 @@
         <v>-5.9475806451613051</v>
       </c>
     </row>
-    <row r="234" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A234" s="7">
         <v>40179</v>
       </c>
@@ -37636,7 +37678,7 @@
         <v>-5.0830227041680782</v>
       </c>
     </row>
-    <row r="235" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A235" s="7">
         <v>40210</v>
       </c>
@@ -37797,7 +37839,7 @@
         <v>-4.267668146124957</v>
       </c>
     </row>
-    <row r="236" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A236" s="7">
         <v>40238</v>
       </c>
@@ -37958,7 +38000,7 @@
         <v>-3.4707903780068805</v>
       </c>
     </row>
-    <row r="237" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A237" s="7">
         <v>40269</v>
       </c>
@@ -38119,7 +38161,7 @@
         <v>-1.8409169850642428</v>
       </c>
     </row>
-    <row r="238" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="7">
         <v>40299</v>
       </c>
@@ -38280,7 +38322,7 @@
         <v>-1.835180055401666</v>
       </c>
     </row>
-    <row r="239" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239" s="7">
         <v>40330</v>
       </c>
@@ -38441,7 +38483,7 @@
         <v>-0.73632538569423778</v>
       </c>
     </row>
-    <row r="240" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A240" s="7">
         <v>40360</v>
       </c>
@@ -38602,7 +38644,7 @@
         <v>-0.67019400352732883</v>
       </c>
     </row>
-    <row r="241" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A241" s="7">
         <v>40391</v>
       </c>
@@ -38763,7 +38805,7 @@
         <v>0.14179369018077889</v>
       </c>
     </row>
-    <row r="242" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A242" s="7">
         <v>40422</v>
       </c>
@@ -38924,7 +38966,7 @@
         <v>0.53059780686239832</v>
       </c>
     </row>
-    <row r="243" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243" s="7">
         <v>40452</v>
       </c>
@@ -39085,7 +39127,7 @@
         <v>1.4250089063056646</v>
       </c>
     </row>
-    <row r="244" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A244" s="7">
         <v>40483</v>
       </c>
@@ -39246,7 +39288,7 @@
         <v>1.1051693404634662</v>
       </c>
     </row>
-    <row r="245" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245" s="7">
         <v>40513</v>
       </c>
@@ -39407,7 +39449,7 @@
         <v>1.2504465880671671</v>
       </c>
     </row>
-    <row r="246" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A246" s="7">
         <v>40544</v>
       </c>
@@ -39568,7 +39610,7 @@
         <v>1.1781506604783842</v>
       </c>
     </row>
-    <row r="247" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247" s="7">
         <v>40575</v>
       </c>
@@ -39729,7 +39771,7 @@
         <v>1.1768901569186918</v>
       </c>
     </row>
-    <row r="248" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A248" s="7">
         <v>40603</v>
       </c>
@@ -39890,7 +39932,7 @@
         <v>1.3171947312210914</v>
       </c>
     </row>
-    <row r="249" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" s="7">
         <v>40634</v>
       </c>
@@ -40051,7 +40093,7 @@
         <v>0.81387119603678493</v>
       </c>
     </row>
-    <row r="250" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A250" s="7">
         <v>40664</v>
       </c>
@@ -40212,7 +40254,7 @@
         <v>0.70546737213403876</v>
       </c>
     </row>
-    <row r="251" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A251" s="7">
         <v>40695</v>
       </c>
@@ -40373,7 +40415,7 @@
         <v>0.98904980572234336</v>
       </c>
     </row>
-    <row r="252" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A252" s="7">
         <v>40725</v>
       </c>
@@ -40534,7 +40576,7 @@
         <v>1.953125</v>
       </c>
     </row>
-    <row r="253" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A253" s="7">
         <v>40756</v>
       </c>
@@ -40695,7 +40737,7 @@
         <v>2.1592920353982379</v>
       </c>
     </row>
-    <row r="254" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A254" s="7">
         <v>40787</v>
       </c>
@@ -40856,7 +40898,7 @@
         <v>1.7945109078114085</v>
       </c>
     </row>
-    <row r="255" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A255" s="7">
         <v>40817</v>
       </c>
@@ -41017,7 +41059,7 @@
         <v>1.5454864769933383</v>
       </c>
     </row>
-    <row r="256" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A256" s="7">
         <v>40848</v>
       </c>
@@ -41178,7 +41220,7 @@
         <v>2.1509167842030905</v>
       </c>
     </row>
-    <row r="257" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" s="7">
         <v>40878</v>
       </c>
@@ -41339,7 +41381,7 @@
         <v>2.3994354269583669</v>
       </c>
     </row>
-    <row r="258" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258" s="7">
         <v>40909</v>
       </c>
@@ -41500,7 +41542,7 @@
         <v>2.3641496118560501</v>
       </c>
     </row>
-    <row r="259" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
         <v>40940</v>
       </c>
@@ -41661,7 +41703,7 @@
         <v>2.3616496298907257</v>
       </c>
     </row>
-    <row r="260" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A260" s="7">
         <v>40969</v>
       </c>
@@ -41822,7 +41864,7 @@
         <v>2.1082220660576247</v>
       </c>
     </row>
-    <row r="261" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="7">
         <v>41000</v>
       </c>
@@ -41983,7 +42025,7 @@
         <v>2.3868023868023909</v>
       </c>
     </row>
-    <row r="262" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A262" s="7">
         <v>41030</v>
       </c>
@@ -42144,7 +42186,7 @@
         <v>1.6112084063047365</v>
       </c>
     </row>
-    <row r="263" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A263" s="7">
         <v>41061</v>
       </c>
@@ -42305,7 +42347,7 @@
         <v>1.1542497376705183</v>
       </c>
     </row>
-    <row r="264" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A264" s="7">
         <v>41091</v>
       </c>
@@ -42466,7 +42508,7 @@
         <v>0.59212817833507081</v>
       </c>
     </row>
-    <row r="265" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A265" s="7">
         <v>41122</v>
       </c>
@@ -42627,7 +42669,7 @@
         <v>0.20790020790019606</v>
       </c>
     </row>
-    <row r="266" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A266" s="7">
         <v>41153</v>
       </c>
@@ -42788,7 +42830,7 @@
         <v>-3.4566194262019616E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A267" s="7">
         <v>41183</v>
       </c>
@@ -42949,7 +42991,7 @@
         <v>6.9180214458660877E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A268" s="7">
         <v>41214</v>
       </c>
@@ -43110,7 +43152,7 @@
         <v>-3.4518467380036555E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A269" s="7">
         <v>41244</v>
       </c>
@@ -43271,7 +43313,7 @@
         <v>-3.4458993797369365E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A270" s="7">
         <v>41275</v>
       </c>
@@ -43432,7 +43474,7 @@
         <v>3.4470872113052706E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A271" s="7">
         <v>41306</v>
       </c>
@@ -43593,7 +43635,7 @@
         <v>-0.20661157024792215</v>
       </c>
     </row>
-    <row r="272" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A272" s="7">
         <v>41334</v>
       </c>
@@ -43754,7 +43796,7 @@
         <v>-0.10323468685478712</v>
       </c>
     </row>
-    <row r="273" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A273" s="7">
         <v>41365</v>
       </c>
@@ -43915,7 +43957,7 @@
         <v>-0.47994514912580644</v>
       </c>
     </row>
-    <row r="274" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A274" s="7">
         <v>41395</v>
       </c>
@@ -44076,7 +44118,7 @@
         <v>0.13788348845224999</v>
       </c>
     </row>
-    <row r="275" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A275" s="7">
         <v>41426</v>
       </c>
@@ -44237,7 +44279,7 @@
         <v>0.82987551867221099</v>
       </c>
     </row>
-    <row r="276" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A276" s="7">
         <v>41456</v>
       </c>
@@ -44398,7 +44440,7 @@
         <v>0.65789473684209732</v>
       </c>
     </row>
-    <row r="277" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A277" s="7">
         <v>41487</v>
       </c>
@@ -44559,7 +44601,7 @@
         <v>0.44951590594744517</v>
       </c>
     </row>
-    <row r="278" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A278" s="7">
         <v>41518</v>
       </c>
@@ -44720,7 +44762,7 @@
         <v>0.41493775933609567</v>
       </c>
     </row>
-    <row r="279" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A279" s="7">
         <v>41548</v>
       </c>
@@ -44881,7 +44923,7 @@
         <v>0.5530591081921763</v>
       </c>
     </row>
-    <row r="280" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A280" s="7">
         <v>41579</v>
       </c>
@@ -45042,7 +45084,7 @@
         <v>0.34530386740331492</v>
       </c>
     </row>
-    <row r="281" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A281" s="7">
         <v>41609</v>
       </c>
@@ -45203,7 +45245,7 @@
         <v>0.27576697690449997</v>
       </c>
     </row>
-    <row r="282" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A282" s="7">
         <v>41640</v>
       </c>
@@ -45364,7 +45406,7 @@
         <v>0.5513439007581058</v>
       </c>
     </row>
-    <row r="283" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A283" s="7">
         <v>41671</v>
       </c>
@@ -45525,7 +45567,7 @@
         <v>0.72463768115940852</v>
       </c>
     </row>
-    <row r="284" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A284" s="7">
         <v>41699</v>
       </c>
@@ -45686,7 +45728,7 @@
         <v>0.68894247330347913</v>
       </c>
     </row>
-    <row r="285" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A285" s="7">
         <v>41730</v>
       </c>
@@ -45847,7 +45889,7 @@
         <v>1.2056493282810885</v>
       </c>
     </row>
-    <row r="286" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A286" s="7">
         <v>41760</v>
       </c>
@@ -46008,7 +46050,7 @@
         <v>1.4802065404475082</v>
       </c>
     </row>
-    <row r="287" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A287" s="7">
         <v>41791</v>
       </c>
@@ -46169,7 +46211,7 @@
         <v>1.2345679012345561</v>
       </c>
     </row>
-    <row r="288" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A288" s="7">
         <v>41821</v>
       </c>
@@ -46330,7 +46372,7 @@
         <v>1.5479876160990713</v>
       </c>
     </row>
-    <row r="289" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A289" s="7">
         <v>41852</v>
       </c>
@@ -46491,7 +46533,7 @@
         <v>1.4457831325301165</v>
       </c>
     </row>
-    <row r="290" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A290" s="7">
         <v>41883</v>
       </c>
@@ -46652,7 +46694,7 @@
         <v>1.721763085399449</v>
       </c>
     </row>
-    <row r="291" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291" s="7">
         <v>41913</v>
       </c>
@@ -46813,7 +46855,7 @@
         <v>1.7875558611206759</v>
       </c>
     </row>
-    <row r="292" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A292" s="7">
         <v>41944</v>
       </c>
@@ -46974,7 +47016,7 @@
         <v>1.6173434273915994</v>
       </c>
     </row>
-    <row r="293" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A293" s="7">
         <v>41974</v>
       </c>
@@ -47135,7 +47177,7 @@
         <v>1.6500515641113827</v>
       </c>
     </row>
-    <row r="294" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A294" s="7">
         <v>42005</v>
       </c>
@@ -47296,7 +47338,7 @@
         <v>1.5421521590130225</v>
       </c>
     </row>
-    <row r="295" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A295" s="7">
         <v>42036</v>
       </c>
@@ -47457,7 +47499,7 @@
         <v>1.301815690304903</v>
       </c>
     </row>
-    <row r="296" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A296" s="7">
         <v>42064</v>
       </c>
@@ -47618,7 +47660,7 @@
         <v>0.88949709202872584</v>
       </c>
     </row>
-    <row r="297" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A297" s="7">
         <v>42095</v>
       </c>
@@ -47779,7 +47821,7 @@
         <v>6.8073519400949148E-2</v>
       </c>
     </row>
-    <row r="298" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298" s="7">
         <v>42125</v>
       </c>
@@ -47940,7 +47982,7 @@
         <v>-0.74626865671641396</v>
       </c>
     </row>
-    <row r="299" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A299" s="7">
         <v>42156</v>
       </c>
@@ -48101,7 +48143,7 @@
         <v>-1.2195121951219396</v>
       </c>
     </row>
-    <row r="300" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A300" s="7">
         <v>42186</v>
       </c>
@@ -48262,7 +48304,7 @@
         <v>-1.1178861788617924</v>
       </c>
     </row>
-    <row r="301" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A301" s="7">
         <v>42217</v>
       </c>
@@ -48423,7 +48465,7 @@
         <v>-0.91618595181540174</v>
       </c>
     </row>
-    <row r="302" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A302" s="7">
         <v>42248</v>
       </c>
@@ -48584,7 +48626,7 @@
         <v>-1.3202437373053411</v>
       </c>
     </row>
-    <row r="303" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A303" s="7">
         <v>42278</v>
       </c>
@@ -48745,7 +48787,7 @@
         <v>-1.8237082066869414</v>
       </c>
     </row>
-    <row r="304" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A304" s="7">
         <v>42309</v>
       </c>
@@ -48906,7 +48948,7 @@
         <v>-2.031832035218422</v>
       </c>
     </row>
-    <row r="305" spans="1:53" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A305" s="7">
         <v>42339</v>
       </c>
@@ -50520,160 +50562,160 @@
       <c r="A315" s="7">
         <v>42644</v>
       </c>
-      <c r="B315" s="9">
+      <c r="B315" s="8">
         <v>1.7057808576598819</v>
       </c>
-      <c r="C315" s="9">
+      <c r="C315" s="8">
         <v>1.2561274509803875</v>
       </c>
-      <c r="D315" s="9">
+      <c r="D315" s="8">
         <v>-2.1604024859425732</v>
       </c>
-      <c r="E315" s="9">
+      <c r="E315" s="8">
         <v>2.6498778425108065</v>
       </c>
-      <c r="F315" s="9">
+      <c r="F315" s="8">
         <v>1.2962507178603622</v>
       </c>
-      <c r="G315" s="9">
+      <c r="G315" s="8">
         <v>2.3157933656648773</v>
       </c>
-      <c r="H315" s="9">
+      <c r="H315" s="8">
         <v>2.4146284285379278</v>
       </c>
-      <c r="I315" s="9">
+      <c r="I315" s="8">
         <v>9.5374344301391065E-2</v>
       </c>
-      <c r="J315" s="9">
+      <c r="J315" s="8">
         <v>0.84425683181514211</v>
       </c>
-      <c r="K315" s="9">
+      <c r="K315" s="8">
         <v>1.3532671736048461</v>
       </c>
-      <c r="L315" s="9">
+      <c r="L315" s="8">
         <v>3.1339170304611854</v>
       </c>
-      <c r="M315" s="9">
+      <c r="M315" s="8">
         <v>2.868108862526173</v>
       </c>
-      <c r="N315" s="9">
+      <c r="N315" s="8">
         <v>1.3549291387634217</v>
       </c>
-      <c r="O315" s="9">
+      <c r="O315" s="8">
         <v>3.6430678466076762</v>
       </c>
-      <c r="P315" s="9">
+      <c r="P315" s="8">
         <v>0.390052006934267</v>
       </c>
-      <c r="Q315" s="9">
+      <c r="Q315" s="8">
         <v>1.7357351445352263</v>
       </c>
-      <c r="R315" s="9">
+      <c r="R315" s="8">
         <v>0.63327576280944742</v>
       </c>
-      <c r="S315" s="9">
+      <c r="S315" s="8">
         <v>0.42665149683566811</v>
       </c>
-      <c r="T315" s="9">
+      <c r="T315" s="8">
         <v>1.3293943870014795</v>
       </c>
-      <c r="U315" s="9">
+      <c r="U315" s="8">
         <v>-1.228932584269663</v>
       </c>
-      <c r="V315" s="9">
+      <c r="V315" s="8">
         <v>0.78534031413611816</v>
       </c>
-      <c r="W315" s="9">
+      <c r="W315" s="8">
         <v>1.1821561338290032</v>
       </c>
-      <c r="X315" s="9">
+      <c r="X315" s="8">
         <v>1.5684937345494789</v>
       </c>
-      <c r="Y315" s="9">
+      <c r="Y315" s="8">
         <v>2.3591210749712603</v>
       </c>
-      <c r="Z315" s="9">
+      <c r="Z315" s="8">
         <v>1.4617128902843219</v>
       </c>
-      <c r="AA315" s="9">
+      <c r="AA315" s="8">
         <v>0.54343062494520267</v>
       </c>
-      <c r="AB315" s="9">
+      <c r="AB315" s="8">
         <v>1.7683056998505757</v>
       </c>
-      <c r="AC315" s="9">
+      <c r="AC315" s="8">
         <v>1.2723743799870679</v>
       </c>
-      <c r="AD315" s="9">
+      <c r="AD315" s="8">
         <v>0.7624517278938554</v>
       </c>
-      <c r="AE315" s="9">
+      <c r="AE315" s="8">
         <v>3.4854445318646698</v>
       </c>
-      <c r="AF315" s="9">
+      <c r="AF315" s="8">
         <v>2.2441243366186434</v>
       </c>
-      <c r="AG315" s="9">
+      <c r="AG315" s="8">
         <v>1.4239017383982964</v>
       </c>
-      <c r="AH315" s="9">
+      <c r="AH315" s="8">
         <v>0.27761013880506391</v>
       </c>
-      <c r="AI315" s="9">
+      <c r="AI315" s="8">
         <v>1.1260318380403358</v>
       </c>
-      <c r="AJ315" s="9">
+      <c r="AJ315" s="8">
         <v>2.1774250193158666</v>
       </c>
-      <c r="AK315" s="9">
+      <c r="AK315" s="8">
         <v>-2.3547880690737837</v>
       </c>
-      <c r="AL315" s="9">
+      <c r="AL315" s="8">
         <v>0.85769908903907977</v>
       </c>
-      <c r="AM315" s="9">
+      <c r="AM315" s="8">
         <v>-0.86413826212194489</v>
       </c>
-      <c r="AN315" s="9">
+      <c r="AN315" s="8">
         <v>2.6942774437764343</v>
       </c>
-      <c r="AO315" s="9">
+      <c r="AO315" s="8">
         <v>1.0519113999828957</v>
       </c>
-      <c r="AP315" s="9">
+      <c r="AP315" s="8">
         <v>0.86242299794660959</v>
       </c>
-      <c r="AQ315" s="9">
+      <c r="AQ315" s="8">
         <v>1.7133264207771712</v>
       </c>
-      <c r="AR315" s="9">
+      <c r="AR315" s="8">
         <v>1.1646866992778944</v>
       </c>
-      <c r="AS315" s="9">
+      <c r="AS315" s="8">
         <v>2.3598314895365995</v>
       </c>
-      <c r="AT315" s="9">
+      <c r="AT315" s="8">
         <v>1.2651011494060114</v>
       </c>
-      <c r="AU315" s="9">
+      <c r="AU315" s="8">
         <v>3.5381082244868631</v>
       </c>
-      <c r="AV315" s="9">
+      <c r="AV315" s="8">
         <v>0.67350865939703841</v>
       </c>
-      <c r="AW315" s="9">
+      <c r="AW315" s="8">
         <v>1.1814866183798223</v>
       </c>
-      <c r="AX315" s="9">
+      <c r="AX315" s="8">
         <v>3.4429388167661648</v>
       </c>
-      <c r="AY315" s="9">
+      <c r="AY315" s="8">
         <v>-1.2844279661017008</v>
       </c>
-      <c r="AZ315" s="9">
+      <c r="AZ315" s="8">
         <v>0.99265846344741071</v>
       </c>
-      <c r="BA315" s="9">
+      <c r="BA315" s="8">
         <v>-4.7127622979016133</v>
       </c>
     </row>
@@ -50681,160 +50723,160 @@
       <c r="A316" s="7">
         <v>42675</v>
       </c>
-      <c r="B316" s="9">
+      <c r="B316" s="8">
         <v>1.6269269002982232</v>
       </c>
-      <c r="C316" s="9">
+      <c r="C316" s="8">
         <v>1.1731701096659015</v>
       </c>
-      <c r="D316" s="9">
+      <c r="D316" s="8">
         <v>-2.1938926771420197</v>
       </c>
-      <c r="E316" s="9">
+      <c r="E316" s="8">
         <v>2.3330832708176974</v>
       </c>
-      <c r="F316" s="9">
+      <c r="F316" s="8">
         <v>1.1065573770491803</v>
       </c>
-      <c r="G316" s="9">
+      <c r="G316" s="8">
         <v>2.3279420721391215</v>
       </c>
-      <c r="H316" s="9">
+      <c r="H316" s="8">
         <v>2.0304766358782458</v>
       </c>
-      <c r="I316" s="9">
+      <c r="I316" s="8">
         <v>-2.9784952641925301E-2</v>
       </c>
-      <c r="J316" s="9">
+      <c r="J316" s="8">
         <v>0.5985369097761003</v>
       </c>
-      <c r="K316" s="9">
+      <c r="K316" s="8">
         <v>1.1844985193768418</v>
       </c>
-      <c r="L316" s="9">
+      <c r="L316" s="8">
         <v>3.0985230657022989</v>
       </c>
-      <c r="M316" s="9">
+      <c r="M316" s="8">
         <v>2.8666341440750935</v>
       </c>
-      <c r="N316" s="9">
+      <c r="N316" s="8">
         <v>1.4795203239370815</v>
       </c>
-      <c r="O316" s="9">
+      <c r="O316" s="8">
         <v>3.644914756025877</v>
       </c>
-      <c r="P316" s="9">
+      <c r="P316" s="8">
         <v>0.33337222675978867</v>
       </c>
-      <c r="Q316" s="9">
+      <c r="Q316" s="8">
         <v>1.7779960707269216</v>
       </c>
-      <c r="R316" s="9">
+      <c r="R316" s="8">
         <v>0.40925949609925127</v>
       </c>
-      <c r="S316" s="9">
+      <c r="S316" s="8">
         <v>0.11370904697605973</v>
       </c>
-      <c r="T316" s="9">
+      <c r="T316" s="8">
         <v>1.3994107744107815</v>
       </c>
-      <c r="U316" s="9">
+      <c r="U316" s="8">
         <v>-1.1961001105638736</v>
       </c>
-      <c r="V316" s="9">
+      <c r="V316" s="8">
         <v>0.83333333333333692</v>
       </c>
-      <c r="W316" s="9">
+      <c r="W316" s="8">
         <v>1.1105746016417053</v>
       </c>
-      <c r="X316" s="9">
+      <c r="X316" s="8">
         <v>1.6307893020221786</v>
       </c>
-      <c r="Y316" s="9">
+      <c r="Y316" s="8">
         <v>2.2807099704959404</v>
       </c>
-      <c r="Z316" s="9">
+      <c r="Z316" s="8">
         <v>1.5322468310349633</v>
       </c>
-      <c r="AA316" s="9">
+      <c r="AA316" s="8">
         <v>0.52594670406732114</v>
       </c>
-      <c r="AB316" s="9">
+      <c r="AB316" s="8">
         <v>1.6972021019741417</v>
       </c>
-      <c r="AC316" s="9">
+      <c r="AC316" s="8">
         <v>1.6580534022394586</v>
       </c>
-      <c r="AD316" s="9">
+      <c r="AD316" s="8">
         <v>1.0582533873998548</v>
       </c>
-      <c r="AE316" s="9">
+      <c r="AE316" s="8">
         <v>3.4352941176470551</v>
       </c>
-      <c r="AF316" s="9">
+      <c r="AF316" s="8">
         <v>2.0121028744326712</v>
       </c>
-      <c r="AG316" s="9">
+      <c r="AG316" s="8">
         <v>1.28122681177344</v>
       </c>
-      <c r="AH316" s="9">
+      <c r="AH316" s="8">
         <v>0.71127185051235409</v>
       </c>
-      <c r="AI316" s="9">
+      <c r="AI316" s="8">
         <v>1.1708446808054265</v>
       </c>
-      <c r="AJ316" s="9">
+      <c r="AJ316" s="8">
         <v>2.2052983226650382</v>
       </c>
-      <c r="AK316" s="9">
+      <c r="AK316" s="8">
         <v>-2.2072072072072095</v>
       </c>
-      <c r="AL316" s="9">
+      <c r="AL316" s="8">
         <v>0.95982675402375128</v>
       </c>
-      <c r="AM316" s="9">
+      <c r="AM316" s="8">
         <v>-0.9370494954348817</v>
       </c>
-      <c r="AN316" s="9">
+      <c r="AN316" s="8">
         <v>2.6191665279396288</v>
       </c>
-      <c r="AO316" s="9">
+      <c r="AO316" s="8">
         <v>1.0423074294306609</v>
       </c>
-      <c r="AP316" s="9">
+      <c r="AP316" s="8">
         <v>0.8813281410125049</v>
       </c>
-      <c r="AQ316" s="9">
+      <c r="AQ316" s="8">
         <v>1.9716088328075823</v>
       </c>
-      <c r="AR316" s="9">
+      <c r="AR316" s="8">
         <v>1.2090211578702599</v>
       </c>
-      <c r="AS316" s="9">
+      <c r="AS316" s="8">
         <v>2.2707065180220263</v>
       </c>
-      <c r="AT316" s="9">
+      <c r="AT316" s="8">
         <v>1.5448060819929179</v>
       </c>
-      <c r="AU316" s="9">
+      <c r="AU316" s="8">
         <v>3.5141711995419342</v>
       </c>
-      <c r="AV316" s="9">
+      <c r="AV316" s="8">
         <v>0.19230769230769962</v>
       </c>
-      <c r="AW316" s="9">
+      <c r="AW316" s="8">
         <v>0.84361137465063429</v>
       </c>
-      <c r="AX316" s="9">
+      <c r="AX316" s="8">
         <v>3.4401285322748261</v>
       </c>
-      <c r="AY316" s="9">
+      <c r="AY316" s="8">
         <v>0.10615711252653325</v>
       </c>
-      <c r="AZ316" s="9">
+      <c r="AZ316" s="8">
         <v>1.109732561345474</v>
       </c>
-      <c r="BA316" s="9">
+      <c r="BA316" s="8">
         <v>-4.3899066712754884</v>
       </c>
     </row>
@@ -50842,160 +50884,160 @@
       <c r="A317" s="7">
         <v>42705</v>
       </c>
-      <c r="B317" s="9">
+      <c r="B317" s="8">
         <v>1.5655030226788273</v>
       </c>
-      <c r="C317" s="9">
+      <c r="C317" s="8">
         <v>1.126631321370317</v>
       </c>
-      <c r="D317" s="9">
+      <c r="D317" s="8">
         <v>-2.1971496437054734</v>
       </c>
-      <c r="E317" s="9">
+      <c r="E317" s="8">
         <v>2.6146978279626469</v>
       </c>
-      <c r="F317" s="9">
+      <c r="F317" s="8">
         <v>1.1940786783348252</v>
       </c>
-      <c r="G317" s="9">
+      <c r="G317" s="8">
         <v>2.1858494042501011</v>
       </c>
-      <c r="H317" s="9">
+      <c r="H317" s="8">
         <v>1.8873064051677171</v>
       </c>
-      <c r="I317" s="9">
+      <c r="I317" s="8">
         <v>-1.1921082434287744E-2</v>
       </c>
-      <c r="J317" s="9">
+      <c r="J317" s="8">
         <v>0.70921985815602584</v>
       </c>
-      <c r="K317" s="9">
+      <c r="K317" s="8">
         <v>1.0910024387113335</v>
       </c>
-      <c r="L317" s="9">
+      <c r="L317" s="8">
         <v>2.9631425800193942</v>
       </c>
-      <c r="M317" s="9">
+      <c r="M317" s="8">
         <v>2.6616057583261972</v>
       </c>
-      <c r="N317" s="9">
+      <c r="N317" s="8">
         <v>1.0854396030392308</v>
       </c>
-      <c r="O317" s="9">
+      <c r="O317" s="8">
         <v>3.8433328443596788</v>
       </c>
-      <c r="P317" s="9">
+      <c r="P317" s="8">
         <v>0.31487405037985716</v>
       </c>
-      <c r="Q317" s="9">
-        <v>1.4644830178810821</v>
-      </c>
-      <c r="R317" s="9">
+      <c r="Q317" s="8">
+        <v>1.6181229773462786</v>
+      </c>
+      <c r="R317" s="8">
         <v>0.40884119074995928</v>
       </c>
-      <c r="S317" s="9">
+      <c r="S317" s="8">
         <v>0.14910536779323408</v>
       </c>
-      <c r="T317" s="9">
+      <c r="T317" s="8">
         <v>1.6313213703099512</v>
       </c>
-      <c r="U317" s="9">
+      <c r="U317" s="8">
         <v>-0.8310249307479225</v>
       </c>
-      <c r="V317" s="9">
+      <c r="V317" s="8">
         <v>0.70112506114463857</v>
       </c>
-      <c r="W317" s="9">
+      <c r="W317" s="8">
         <v>1.3133486681012128</v>
       </c>
-      <c r="X317" s="9">
+      <c r="X317" s="8">
         <v>1.5862225243598458</v>
       </c>
-      <c r="Y317" s="9">
+      <c r="Y317" s="8">
         <v>2.1606453875832954</v>
       </c>
-      <c r="Z317" s="9">
+      <c r="Z317" s="8">
         <v>1.7271397729646878</v>
       </c>
-      <c r="AA317" s="9">
+      <c r="AA317" s="8">
         <v>0.15745276417074477</v>
       </c>
-      <c r="AB317" s="9">
+      <c r="AB317" s="8">
         <v>1.8369445725025615</v>
       </c>
-      <c r="AC317" s="9">
+      <c r="AC317" s="8">
         <v>1.4626801462680172</v>
       </c>
-      <c r="AD317" s="9">
+      <c r="AD317" s="8">
         <v>0.98823994465856313</v>
       </c>
-      <c r="AE317" s="9">
+      <c r="AE317" s="8">
         <v>3.2184985548004099</v>
       </c>
-      <c r="AF317" s="9">
+      <c r="AF317" s="8">
         <v>1.8137847642079805</v>
       </c>
-      <c r="AG317" s="9">
+      <c r="AG317" s="8">
         <v>1.4561906645569529</v>
       </c>
-      <c r="AH317" s="9">
+      <c r="AH317" s="8">
         <v>1.0755287009063417</v>
       </c>
-      <c r="AI317" s="9">
+      <c r="AI317" s="8">
         <v>1.343633811569819</v>
       </c>
-      <c r="AJ317" s="9">
+      <c r="AJ317" s="8">
         <v>2.1918063748921588</v>
       </c>
-      <c r="AK317" s="9">
+      <c r="AK317" s="8">
         <v>-1.9217725525661316</v>
       </c>
-      <c r="AL317" s="9">
+      <c r="AL317" s="8">
         <v>0.91125779244590788</v>
       </c>
-      <c r="AM317" s="9">
+      <c r="AM317" s="8">
         <v>-0.75775799855664605</v>
       </c>
-      <c r="AN317" s="9">
+      <c r="AN317" s="8">
         <v>2.5520372010628822</v>
       </c>
-      <c r="AO317" s="9">
+      <c r="AO317" s="8">
         <v>1.0400655804898136</v>
       </c>
-      <c r="AP317" s="9">
+      <c r="AP317" s="8">
         <v>0.55259926320098007</v>
       </c>
-      <c r="AQ317" s="9">
+      <c r="AQ317" s="8">
         <v>1.7893132772943945</v>
       </c>
-      <c r="AR317" s="9">
+      <c r="AR317" s="8">
         <v>1.1147236414305512</v>
       </c>
-      <c r="AS317" s="9">
+      <c r="AS317" s="8">
         <v>2.1493637201050801</v>
       </c>
-      <c r="AT317" s="9">
+      <c r="AT317" s="8">
         <v>1.6225720026791635</v>
       </c>
-      <c r="AU317" s="9">
+      <c r="AU317" s="8">
         <v>3.5063914875383948</v>
       </c>
-      <c r="AV317" s="9">
+      <c r="AV317" s="8">
         <v>0.70580686557587058</v>
       </c>
-      <c r="AW317" s="9">
+      <c r="AW317" s="8">
         <v>0.85835810187557637</v>
       </c>
-      <c r="AX317" s="9">
+      <c r="AX317" s="8">
         <v>3.4412319296040224</v>
       </c>
-      <c r="AY317" s="9">
+      <c r="AY317" s="8">
         <v>-0.79702444208289058</v>
       </c>
-      <c r="AZ317" s="9">
+      <c r="AZ317" s="8">
         <v>0.90787165996079955</v>
       </c>
-      <c r="BA317" s="9">
+      <c r="BA317" s="8">
         <v>-3.9555863983344821</v>
       </c>
     </row>
@@ -51003,160 +51045,160 @@
       <c r="A318" s="7">
         <v>42736</v>
       </c>
-      <c r="B318" s="9">
-        <v>1.6423319437752686</v>
-      </c>
-      <c r="C318" s="9">
+      <c r="B318" s="8">
+        <v>1.6269699953215884</v>
+      </c>
+      <c r="C318" s="8">
         <v>1.4286440591794147</v>
       </c>
-      <c r="D318" s="9">
+      <c r="D318" s="8">
         <v>-2.4085637823372053</v>
       </c>
-      <c r="E318" s="9">
+      <c r="E318" s="8">
         <v>2.1811515582326209</v>
       </c>
-      <c r="F318" s="9">
+      <c r="F318" s="8">
         <v>1.0804616517966805</v>
       </c>
-      <c r="G318" s="9">
+      <c r="G318" s="8">
         <v>2.0591768195523739</v>
       </c>
-      <c r="H318" s="9">
+      <c r="H318" s="8">
         <v>2.0768633540372674</v>
       </c>
-      <c r="I318" s="9">
+      <c r="I318" s="8">
         <v>0.36953152938371947</v>
       </c>
-      <c r="J318" s="9">
+      <c r="J318" s="8">
         <v>0.97474523704032656</v>
       </c>
-      <c r="K318" s="9">
+      <c r="K318" s="8">
         <v>1.2340917855765552</v>
       </c>
-      <c r="L318" s="9">
+      <c r="L318" s="8">
         <v>3.3765479876161084</v>
       </c>
-      <c r="M318" s="9">
+      <c r="M318" s="8">
         <v>2.6042749855574772</v>
       </c>
-      <c r="N318" s="9">
+      <c r="N318" s="8">
         <v>1.1515717398070304</v>
       </c>
-      <c r="O318" s="9">
+      <c r="O318" s="8">
         <v>4.0274332409163911</v>
       </c>
-      <c r="P318" s="9">
+      <c r="P318" s="8">
         <v>0.37122738093255103</v>
       </c>
-      <c r="Q318" s="9">
-        <v>1.3110263183641462</v>
-      </c>
-      <c r="R318" s="9">
+      <c r="Q318" s="8">
+        <v>1.4675667742882301</v>
+      </c>
+      <c r="R318" s="8">
         <v>0.58024612637889028</v>
       </c>
-      <c r="S318" s="9">
+      <c r="S318" s="8">
         <v>-0.17028522775649857</v>
       </c>
-      <c r="T318" s="9">
+      <c r="T318" s="8">
         <v>1.5753820301423096</v>
       </c>
-      <c r="U318" s="9">
+      <c r="U318" s="8">
         <v>-0.3430012610340456</v>
       </c>
-      <c r="V318" s="9">
+      <c r="V318" s="8">
         <v>1.0069839207406093</v>
       </c>
-      <c r="W318" s="9">
+      <c r="W318" s="8">
         <v>1.7238183503243742</v>
       </c>
-      <c r="X318" s="9">
+      <c r="X318" s="8">
         <v>1.6750134397193168</v>
       </c>
-      <c r="Y318" s="9">
+      <c r="Y318" s="8">
         <v>2.067647264505017</v>
       </c>
-      <c r="Z318" s="9">
+      <c r="Z318" s="8">
         <v>1.273951680088858</v>
       </c>
-      <c r="AA318" s="9">
+      <c r="AA318" s="8">
         <v>9.6027935399380968E-2</v>
       </c>
-      <c r="AB318" s="9">
+      <c r="AB318" s="8">
         <v>1.8839861179970188</v>
       </c>
-      <c r="AC318" s="9">
+      <c r="AC318" s="8">
         <v>1.9123334765792941</v>
       </c>
-      <c r="AD318" s="9">
+      <c r="AD318" s="8">
         <v>0.82137555665511663</v>
       </c>
-      <c r="AE318" s="9">
+      <c r="AE318" s="8">
         <v>3.4118475624070665</v>
       </c>
-      <c r="AF318" s="9">
+      <c r="AF318" s="8">
         <v>2.4853140533212836</v>
       </c>
-      <c r="AG318" s="9">
+      <c r="AG318" s="8">
         <v>1.7545593831858959</v>
       </c>
-      <c r="AH318" s="9">
+      <c r="AH318" s="8">
         <v>0.6035003017501509</v>
       </c>
-      <c r="AI318" s="9">
+      <c r="AI318" s="8">
         <v>1.4688890790824982</v>
       </c>
-      <c r="AJ318" s="9">
+      <c r="AJ318" s="8">
         <v>1.8641346086713764</v>
       </c>
-      <c r="AK318" s="9">
+      <c r="AK318" s="8">
         <v>-0.68446269678302529</v>
       </c>
-      <c r="AL318" s="9">
+      <c r="AL318" s="8">
         <v>0.6635590896627398</v>
       </c>
-      <c r="AM318" s="9">
+      <c r="AM318" s="8">
         <v>-0.54161400974905216</v>
       </c>
-      <c r="AN318" s="9">
+      <c r="AN318" s="8">
         <v>2.2793752414592392</v>
       </c>
-      <c r="AO318" s="9">
+      <c r="AO318" s="8">
         <v>1.1567399723610834</v>
       </c>
-      <c r="AP318" s="9">
+      <c r="AP318" s="8">
         <v>1.0038926449498007</v>
       </c>
-      <c r="AQ318" s="9">
+      <c r="AQ318" s="8">
         <v>1.9945959223777898</v>
       </c>
-      <c r="AR318" s="9">
+      <c r="AR318" s="8">
         <v>1.0223048327137627</v>
       </c>
-      <c r="AS318" s="9">
+      <c r="AS318" s="8">
         <v>2.2509790567001504</v>
       </c>
-      <c r="AT318" s="9">
+      <c r="AT318" s="8">
         <v>1.9032414450258341</v>
       </c>
-      <c r="AU318" s="9">
+      <c r="AU318" s="8">
         <v>3.2797381900967655</v>
       </c>
-      <c r="AV318" s="9">
+      <c r="AV318" s="8">
         <v>1.1527377521613722</v>
       </c>
-      <c r="AW318" s="9">
+      <c r="AW318" s="8">
         <v>1.3378871141698006</v>
       </c>
-      <c r="AX318" s="9">
+      <c r="AX318" s="8">
         <v>2.958765146059676</v>
       </c>
-      <c r="AY318" s="9">
+      <c r="AY318" s="8">
         <v>-0.67846215245443964</v>
       </c>
-      <c r="AZ318" s="9">
+      <c r="AZ318" s="8">
         <v>0.72985197368420118</v>
       </c>
-      <c r="BA318" s="9">
+      <c r="BA318" s="8">
         <v>-3.2044583768721857</v>
       </c>
     </row>
@@ -51164,161 +51206,644 @@
       <c r="A319" s="7">
         <v>42767</v>
       </c>
-      <c r="B319" s="9">
-        <v>1.6382243042775084</v>
-      </c>
-      <c r="C319" s="9">
-        <v>1.4790343074968186</v>
-      </c>
-      <c r="D319" s="9">
-        <v>-1.9940476190476157</v>
-      </c>
-      <c r="E319" s="9">
-        <v>2.1709127531798953</v>
-      </c>
-      <c r="F319" s="9">
-        <v>1.3309381889442276</v>
-      </c>
-      <c r="G319" s="9">
-        <v>1.9302824520332713</v>
-      </c>
-      <c r="H319" s="9">
-        <v>1.9487060282039435</v>
-      </c>
-      <c r="I319" s="9">
-        <v>0.12497768255669442</v>
-      </c>
-      <c r="J319" s="9">
-        <v>0.6634232640424591</v>
-      </c>
-      <c r="K319" s="9">
-        <v>0.53777208706786761</v>
-      </c>
-      <c r="L319" s="9">
-        <v>2.9996865279351743</v>
-      </c>
-      <c r="M319" s="9">
-        <v>2.6278179890277071</v>
-      </c>
-      <c r="N319" s="9">
-        <v>0.77459333849728895</v>
-      </c>
-      <c r="O319" s="9">
-        <v>3.5589773387565367</v>
-      </c>
-      <c r="P319" s="9">
-        <v>0.7822902796271638</v>
-      </c>
-      <c r="Q319" s="9">
-        <v>1.281550871714809</v>
-      </c>
-      <c r="R319" s="9">
-        <v>0.69448869066582297</v>
-      </c>
-      <c r="S319" s="9">
-        <v>-2.8336639274572369E-2</v>
-      </c>
-      <c r="T319" s="9">
+      <c r="B319" s="8">
+        <v>1.6207963861468964</v>
+      </c>
+      <c r="C319" s="8">
+        <v>1.5146124523506965</v>
+      </c>
+      <c r="D319" s="8">
+        <v>-1.755952380952374</v>
+      </c>
+      <c r="E319" s="8">
+        <v>2.2007534783095228</v>
+      </c>
+      <c r="F319" s="8">
+        <v>1.2982771290928279</v>
+      </c>
+      <c r="G319" s="8">
+        <v>1.9217251517392804</v>
+      </c>
+      <c r="H319" s="8">
+        <v>2.0610568727723648</v>
+      </c>
+      <c r="I319" s="8">
+        <v>0.22615009224542965</v>
+      </c>
+      <c r="J319" s="8">
+        <v>0.95090667846086052</v>
+      </c>
+      <c r="K319" s="8">
+        <v>0.93469910371318243</v>
+      </c>
+      <c r="L319" s="8">
+        <v>3.0575582937474204</v>
+      </c>
+      <c r="M319" s="8">
+        <v>2.729242542990193</v>
+      </c>
+      <c r="N319" s="8">
+        <v>0.74360960495739026</v>
+      </c>
+      <c r="O319" s="8">
+        <v>3.3265543288785562</v>
+      </c>
+      <c r="P319" s="8">
+        <v>0.60252996005325932</v>
+      </c>
+      <c r="Q319" s="8">
+        <v>1.466952901379128</v>
+      </c>
+      <c r="R319" s="8">
+        <v>0.73908888180948762</v>
+      </c>
+      <c r="S319" s="8">
+        <v>7.0841598186455093E-2</v>
+      </c>
+      <c r="T319" s="8">
         <v>1.3823437009110948</v>
       </c>
-      <c r="U319" s="9">
-        <v>0.15156107911488331</v>
-      </c>
-      <c r="V319" s="9">
-        <v>0.46978778551759132</v>
-      </c>
-      <c r="W319" s="9">
-        <v>2.1425658894613999</v>
-      </c>
-      <c r="X319" s="9">
-        <v>1.6272314504075076</v>
-      </c>
-      <c r="Y319" s="9">
-        <v>1.9234351713859996</v>
-      </c>
-      <c r="Z319" s="9">
-        <v>1.2792955207322179</v>
-      </c>
-      <c r="AA319" s="9">
-        <v>6.9741086217433704E-2</v>
-      </c>
-      <c r="AB319" s="9">
-        <v>1.9104900053069169</v>
-      </c>
-      <c r="AC319" s="9">
-        <v>2.4248927038626631</v>
-      </c>
-      <c r="AD319" s="9">
-        <v>1.3450697260409479</v>
-      </c>
-      <c r="AE319" s="9">
-        <v>3.2102228455664497</v>
-      </c>
-      <c r="AF319" s="9">
-        <v>1.665666266506606</v>
-      </c>
-      <c r="AG319" s="9">
-        <v>1.8168371749044696</v>
-      </c>
-      <c r="AH319" s="9">
-        <v>0.70939040519417784</v>
-      </c>
-      <c r="AI319" s="9">
-        <v>1.4441821464050215</v>
-      </c>
-      <c r="AJ319" s="9">
-        <v>1.7821920033416143</v>
-      </c>
-      <c r="AK319" s="9">
-        <v>-0.68634179821551122</v>
-      </c>
-      <c r="AL319" s="9">
-        <v>0.82898148486286438</v>
-      </c>
-      <c r="AM319" s="9">
-        <v>-0.42102730662817278</v>
-      </c>
-      <c r="AN319" s="9">
-        <v>2.1905023332418385</v>
-      </c>
-      <c r="AO319" s="9">
-        <v>1.2611629967959641</v>
-      </c>
-      <c r="AP319" s="9">
-        <v>1.2058042100960509</v>
-      </c>
-      <c r="AQ319" s="9">
-        <v>1.5668608921314318</v>
-      </c>
-      <c r="AR319" s="9">
-        <v>1.3704994192799018</v>
-      </c>
-      <c r="AS319" s="9">
-        <v>2.2446346101602797</v>
-      </c>
-      <c r="AT319" s="9">
-        <v>1.8570784415237518</v>
-      </c>
-      <c r="AU319" s="9">
-        <v>3.2530120481927778</v>
-      </c>
-      <c r="AV319" s="9">
-        <v>1.0879999999999928</v>
-      </c>
-      <c r="AW319" s="9">
-        <v>1.3703191434865016</v>
-      </c>
-      <c r="AX319" s="9">
-        <v>2.741221231210631</v>
-      </c>
-      <c r="AY319" s="9">
-        <v>-0.35952063914780902</v>
-      </c>
-      <c r="AZ319" s="9">
+      <c r="U319" s="8">
+        <v>0.21218551076082739</v>
+      </c>
+      <c r="V319" s="8">
+        <v>0.43738862789568206</v>
+      </c>
+      <c r="W319" s="8">
+        <v>2.0684286614523555</v>
+      </c>
+      <c r="X319" s="8">
+        <v>1.6582531938294856</v>
+      </c>
+      <c r="Y319" s="8">
+        <v>1.900149031296581</v>
+      </c>
+      <c r="Z319" s="8">
+        <v>1.3625017334627558</v>
+      </c>
+      <c r="AA319" s="8">
+        <v>-7.8458721994583189E-2</v>
+      </c>
+      <c r="AB319" s="8">
+        <v>1.9140279497611854</v>
+      </c>
+      <c r="AC319" s="8">
+        <v>2.3605150214592276</v>
+      </c>
+      <c r="AD319" s="8">
+        <v>1.3747403817624346</v>
+      </c>
+      <c r="AE319" s="8">
+        <v>3.3115162848683184</v>
+      </c>
+      <c r="AF319" s="8">
+        <v>1.740696278511408</v>
+      </c>
+      <c r="AG319" s="8">
+        <v>1.7749291260939233</v>
+      </c>
+      <c r="AH319" s="8">
+        <v>0.63724900805578388</v>
+      </c>
+      <c r="AI319" s="8">
+        <v>1.4559321490754804</v>
+      </c>
+      <c r="AJ319" s="8">
+        <v>1.8053976283851247</v>
+      </c>
+      <c r="AK319" s="8">
+        <v>-0.66346373827500205</v>
+      </c>
+      <c r="AL319" s="8">
+        <v>0.84358908812036326</v>
+      </c>
+      <c r="AM319" s="8">
+        <v>-0.39696860339227169</v>
+      </c>
+      <c r="AN319" s="8">
+        <v>2.1575624485314275</v>
+      </c>
+      <c r="AO319" s="8">
+        <v>1.4094348626354867</v>
+      </c>
+      <c r="AP319" s="8">
+        <v>1.226241569589209</v>
+      </c>
+      <c r="AQ319" s="8">
+        <v>1.6647896978896455</v>
+      </c>
+      <c r="AR319" s="8">
+        <v>1.4634146341463441</v>
+      </c>
+      <c r="AS319" s="8">
+        <v>2.0816354251561981</v>
+      </c>
+      <c r="AT319" s="8">
+        <v>1.9188697206032259</v>
+      </c>
+      <c r="AU319" s="8">
+        <v>3.2175761871013528</v>
+      </c>
+      <c r="AV319" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="AW319" s="8">
+        <v>1.4369140925157615</v>
+      </c>
+      <c r="AX319" s="8">
+        <v>2.7536955030250168</v>
+      </c>
+      <c r="AY319" s="8">
+        <v>-0.41278295605859155</v>
+      </c>
+      <c r="AZ319" s="8">
         <v>0.9648942722233721</v>
       </c>
-      <c r="BA319" s="9">
-        <v>-2.52100840336136</v>
+      <c r="BA319" s="8">
+        <v>-2.7661064425770423</v>
+      </c>
+    </row>
+    <row r="320" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A320" s="7">
+        <v>42795</v>
+      </c>
+      <c r="B320" s="8">
+        <v>1.496453752618794</v>
+      </c>
+      <c r="C320" s="8">
+        <v>1.5246226558926665</v>
+      </c>
+      <c r="D320" s="8">
+        <v>-2.0578586340590617</v>
+      </c>
+      <c r="E320" s="8">
+        <v>1.9031657355679668</v>
+      </c>
+      <c r="F320" s="8">
+        <v>1.108846310640025</v>
+      </c>
+      <c r="G320" s="8">
+        <v>2.14037534561648</v>
+      </c>
+      <c r="H320" s="8">
+        <v>1.8875952500676796</v>
+      </c>
+      <c r="I320" s="8">
+        <v>5.3450528566343442E-2</v>
+      </c>
+      <c r="J320" s="8">
+        <v>0.61769247738804578</v>
+      </c>
+      <c r="K320" s="8">
+        <v>0.96006144393241155</v>
+      </c>
+      <c r="L320" s="8">
+        <v>2.8129852309247911</v>
+      </c>
+      <c r="M320" s="8">
+        <v>3.100274503471653</v>
+      </c>
+      <c r="N320" s="8">
+        <v>0.69702602230483268</v>
+      </c>
+      <c r="O320" s="8">
+        <v>2.6506373117033704</v>
+      </c>
+      <c r="P320" s="8">
+        <v>0.44427435189190684</v>
+      </c>
+      <c r="Q320" s="8">
+        <v>1.4182551558129064</v>
+      </c>
+      <c r="R320" s="8">
+        <v>0.48966613672496317</v>
+      </c>
+      <c r="S320" s="8">
+        <v>0.22688598979011756</v>
+      </c>
+      <c r="T320" s="8">
+        <v>1.5875510845646117</v>
+      </c>
+      <c r="U320" s="8">
+        <v>-0.15680323722811881</v>
+      </c>
+      <c r="V320" s="8">
+        <v>0.8418326048243373</v>
+      </c>
+      <c r="W320" s="8">
+        <v>1.609858998556678</v>
+      </c>
+      <c r="X320" s="8">
+        <v>1.4033015551618462</v>
+      </c>
+      <c r="Y320" s="8">
+        <v>1.8563751831949238</v>
+      </c>
+      <c r="Z320" s="8">
+        <v>1.5460879814192243</v>
+      </c>
+      <c r="AA320" s="8">
+        <v>-6.1082024432813749E-2</v>
+      </c>
+      <c r="AB320" s="8">
+        <v>1.3150917382543315</v>
+      </c>
+      <c r="AC320" s="8">
+        <v>2.2084048027444276</v>
+      </c>
+      <c r="AD320" s="8">
+        <v>0.86785009861932494</v>
+      </c>
+      <c r="AE320" s="8">
+        <v>3.1271878646441111</v>
+      </c>
+      <c r="AF320" s="8">
+        <v>1.5183403487672742</v>
+      </c>
+      <c r="AG320" s="8">
+        <v>1.346859380001473</v>
+      </c>
+      <c r="AH320" s="8">
+        <v>0.92815814850529554</v>
+      </c>
+      <c r="AI320" s="8">
+        <v>1.0778826163441586</v>
+      </c>
+      <c r="AJ320" s="8">
+        <v>1.6118946710206437</v>
+      </c>
+      <c r="AK320" s="8">
+        <v>-0.27535566773749165</v>
+      </c>
+      <c r="AL320" s="8">
+        <v>0.66214293531794133</v>
+      </c>
+      <c r="AM320" s="8">
+        <v>-0.13874645593291637</v>
+      </c>
+      <c r="AN320" s="8">
+        <v>2.1056094752426309</v>
+      </c>
+      <c r="AO320" s="8">
+        <v>0.95682375374557016</v>
+      </c>
+      <c r="AP320" s="8">
+        <v>0.85609457806766986</v>
+      </c>
+      <c r="AQ320" s="8">
+        <v>1.5916548312845877</v>
+      </c>
+      <c r="AR320" s="8">
+        <v>1.6705336426914126</v>
+      </c>
+      <c r="AS320" s="8">
+        <v>2.2092708050962413</v>
+      </c>
+      <c r="AT320" s="8">
+        <v>2.1026065301142425</v>
+      </c>
+      <c r="AU320" s="8">
+        <v>3.1375874496502081</v>
+      </c>
+      <c r="AV320" s="8">
+        <v>0.9939083039435791</v>
+      </c>
+      <c r="AW320" s="8">
+        <v>1.1715053075840949</v>
+      </c>
+      <c r="AX320" s="8">
+        <v>2.9067596165816041</v>
+      </c>
+      <c r="AY320" s="8">
+        <v>-0.73157754722000534</v>
+      </c>
+      <c r="AZ320" s="8">
+        <v>0.82449538145740364</v>
+      </c>
+      <c r="BA320" s="8">
+        <v>-2.2136331693605098</v>
+      </c>
+    </row>
+    <row r="321" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A321" s="7">
+        <v>42826</v>
+      </c>
+      <c r="B321" s="8">
+        <v>1.5094628231335085</v>
+      </c>
+      <c r="C321" s="8">
+        <v>1.2981744421906649</v>
+      </c>
+      <c r="D321" s="8">
+        <v>-1.9994031632348686</v>
+      </c>
+      <c r="E321" s="8">
+        <v>1.8569412463789645</v>
+      </c>
+      <c r="F321" s="8">
+        <v>1.5098343262874399</v>
+      </c>
+      <c r="G321" s="8">
+        <v>1.4314816503998387</v>
+      </c>
+      <c r="H321" s="8">
+        <v>1.7295961701799158</v>
+      </c>
+      <c r="I321" s="8">
+        <v>0.23246110746855003</v>
+      </c>
+      <c r="J321" s="8">
+        <v>0.59602649006622266</v>
+      </c>
+      <c r="K321" s="8">
+        <v>0.51105148843746007</v>
+      </c>
+      <c r="L321" s="8">
+        <v>2.5824327404013294</v>
+      </c>
+      <c r="M321" s="8">
+        <v>2.6647676368564928</v>
+      </c>
+      <c r="N321" s="8">
+        <v>1.3186472230840831</v>
+      </c>
+      <c r="O321" s="8">
+        <v>2.6604973973394994</v>
+      </c>
+      <c r="P321" s="8">
+        <v>0.36622719403382609</v>
+      </c>
+      <c r="Q321" s="8">
+        <v>1.1575729986343211</v>
+      </c>
+      <c r="R321" s="8">
+        <v>0.37538970541451061</v>
+      </c>
+      <c r="S321" s="8">
+        <v>-0.12045631687097325</v>
+      </c>
+      <c r="T321" s="8">
+        <v>1.6349630561232535</v>
+      </c>
+      <c r="U321" s="8">
+        <v>-0.15184491572607178</v>
+      </c>
+      <c r="V321" s="8">
+        <v>0.63106796116504482</v>
+      </c>
+      <c r="W321" s="8">
+        <v>1.5347065567101807</v>
+      </c>
+      <c r="X321" s="8">
+        <v>1.5178395426769196</v>
+      </c>
+      <c r="Y321" s="8">
+        <v>1.7308494369525886</v>
+      </c>
+      <c r="Z321" s="8">
+        <v>1.7477807329625887</v>
+      </c>
+      <c r="AA321" s="8">
+        <v>7.8657577346605806E-2</v>
+      </c>
+      <c r="AB321" s="8">
+        <v>1.3062665489849956</v>
+      </c>
+      <c r="AC321" s="8">
+        <v>1.7112299465240641</v>
+      </c>
+      <c r="AD321" s="8">
+        <v>1.2055335968379493</v>
+      </c>
+      <c r="AE321" s="8">
+        <v>3.3157731639293426</v>
+      </c>
+      <c r="AF321" s="8">
+        <v>1.8004501125281318</v>
+      </c>
+      <c r="AG321" s="8">
+        <v>1.2942594916463648</v>
+      </c>
+      <c r="AH321" s="8">
+        <v>1.1438892233594222</v>
+      </c>
+      <c r="AI321" s="8">
+        <v>1.0289293170295297</v>
+      </c>
+      <c r="AJ321" s="8">
+        <v>1.1993899057127138</v>
+      </c>
+      <c r="AK321" s="8">
+        <v>0.34443168771526977</v>
+      </c>
+      <c r="AL321" s="8">
+        <v>0.58792382552175004</v>
+      </c>
+      <c r="AM321" s="8">
+        <v>-0.16318143357910178</v>
+      </c>
+      <c r="AN321" s="8">
+        <v>2.3101768215908494</v>
+      </c>
+      <c r="AO321" s="8">
+        <v>0.79263832899592546</v>
+      </c>
+      <c r="AP321" s="8">
+        <v>1.0620915032679714</v>
+      </c>
+      <c r="AQ321" s="8">
+        <v>1.2600732600732689</v>
+      </c>
+      <c r="AR321" s="8">
+        <v>1.6913809082483675</v>
+      </c>
+      <c r="AS321" s="8">
+        <v>1.9603859827323544</v>
+      </c>
+      <c r="AT321" s="8">
+        <v>2.1477663230240549</v>
+      </c>
+      <c r="AU321" s="8">
+        <v>3.1708004509582861</v>
+      </c>
+      <c r="AV321" s="8">
+        <v>1.0262989095574049</v>
+      </c>
+      <c r="AW321" s="8">
+        <v>1.0918202971183057</v>
+      </c>
+      <c r="AX321" s="8">
+        <v>2.5758655962307402</v>
+      </c>
+      <c r="AY321" s="8">
+        <v>-0.32021347565043057</v>
+      </c>
+      <c r="AZ321" s="8">
+        <v>1.2276442225489737</v>
+      </c>
+      <c r="BA321" s="8">
+        <v>-1.3069586718474195</v>
+      </c>
+    </row>
+    <row r="322" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A322" s="7">
+        <v>42856</v>
+      </c>
+      <c r="B322" s="8">
+        <v>1.5750439636057803</v>
+      </c>
+      <c r="C322" s="8">
+        <v>1.8159683473673507</v>
+      </c>
+      <c r="D322" s="8">
+        <v>-0.86930455635492632</v>
+      </c>
+      <c r="E322" s="8">
+        <v>1.8291099321040227</v>
+      </c>
+      <c r="F322" s="8">
+        <v>1.7963582918265699</v>
+      </c>
+      <c r="G322" s="8">
+        <v>1.4743328734905623</v>
+      </c>
+      <c r="H322" s="8">
+        <v>2.3997522836352378</v>
+      </c>
+      <c r="I322" s="8">
+        <v>0.65581589459249989</v>
+      </c>
+      <c r="J322" s="8">
+        <v>0.8855435023245517</v>
+      </c>
+      <c r="K322" s="8">
+        <v>1.4329580348004007</v>
+      </c>
+      <c r="L322" s="8">
+        <v>2.7292315058654539</v>
+      </c>
+      <c r="M322" s="8">
+        <v>2.3634863142451139</v>
+      </c>
+      <c r="N322" s="8">
+        <v>1.2538699690402511</v>
+      </c>
+      <c r="O322" s="8">
+        <v>2.4277456647398781</v>
+      </c>
+      <c r="P322" s="8">
+        <v>0.57863229335157718</v>
+      </c>
+      <c r="Q322" s="8">
+        <v>1.3570243092843834</v>
+      </c>
+      <c r="R322" s="8">
+        <v>0.96944958224375388</v>
+      </c>
+      <c r="S322" s="8">
+        <v>-0.2627281119079774</v>
+      </c>
+      <c r="T322" s="8">
+        <v>1.3814033802522157</v>
+      </c>
+      <c r="U322" s="8">
+        <v>0.47623872732800138</v>
+      </c>
+      <c r="V322" s="8">
+        <v>0.55185846453497445</v>
+      </c>
+      <c r="W322" s="8">
+        <v>1.5957643748380137</v>
+      </c>
+      <c r="X322" s="8">
+        <v>1.6424385846292591</v>
+      </c>
+      <c r="Y322" s="8">
+        <v>1.7269393250081366</v>
+      </c>
+      <c r="Z322" s="8">
+        <v>1.6500622665006164</v>
+      </c>
+      <c r="AA322" s="8">
+        <v>0.22769069095366573</v>
+      </c>
+      <c r="AB322" s="8">
+        <v>1.6603080401299986</v>
+      </c>
+      <c r="AC322" s="8">
+        <v>1.5828877005347544</v>
+      </c>
+      <c r="AD322" s="8">
+        <v>1.1543014996053602</v>
+      </c>
+      <c r="AE322" s="8">
+        <v>2.7087686711554837</v>
+      </c>
+      <c r="AF322" s="8">
+        <v>1.428141912206855</v>
+      </c>
+      <c r="AG322" s="8">
+        <v>1.0614456347740517</v>
+      </c>
+      <c r="AH322" s="8">
+        <v>0.89210367691380066</v>
+      </c>
+      <c r="AI322" s="8">
+        <v>1.5923362809175996</v>
+      </c>
+      <c r="AJ322" s="8">
+        <v>1.598632383856581</v>
+      </c>
+      <c r="AK322" s="8">
+        <v>1.1062456787278201</v>
+      </c>
+      <c r="AL322" s="8">
+        <v>0.75078092176167643</v>
+      </c>
+      <c r="AM322" s="8">
+        <v>0.1454369167373569</v>
+      </c>
+      <c r="AN322" s="8">
+        <v>2.368061252392669</v>
+      </c>
+      <c r="AO322" s="8">
+        <v>0.92029244848918657</v>
+      </c>
+      <c r="AP322" s="8">
+        <v>1.4540241654720387</v>
+      </c>
+      <c r="AQ322" s="8">
+        <v>1.5965237769749181</v>
+      </c>
+      <c r="AR322" s="8">
+        <v>1.2508686587908349</v>
+      </c>
+      <c r="AS322" s="8">
+        <v>1.946710904966652</v>
+      </c>
+      <c r="AT322" s="8">
+        <v>2.222611276459165</v>
+      </c>
+      <c r="AU322" s="8">
+        <v>3.2775355183570221</v>
+      </c>
+      <c r="AV322" s="8">
+        <v>0.54487179487179116</v>
+      </c>
+      <c r="AW322" s="8">
+        <v>1.1363927209439251</v>
+      </c>
+      <c r="AX322" s="8">
+        <v>2.3554868624420346</v>
+      </c>
+      <c r="AY322" s="8">
+        <v>-0.97294415567105896</v>
+      </c>
+      <c r="AZ322" s="8">
+        <v>1.3851270271196932</v>
+      </c>
+      <c r="BA322" s="8">
+        <v>-1.3839602555003669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>